<commit_message>
Fixed excel report export: added styles for comparison analysis and fixed the way distributed params are exported.
</commit_message>
<xml_diff>
--- a/Шаблон отчёта.xlsx
+++ b/Шаблон отчёта.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACA183C-0019-477A-9C9D-2EDC7F21C0F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C52728-147E-4D94-A6CF-D5BF90CA6B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1528,7 +1528,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1645,9 +1645,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1690,6 +1687,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1715,9 +1715,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2159,8 +2156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A200" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="M164" sqref="M164"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2288,21 +2285,21 @@
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44" t="s">
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="44"/>
-      <c r="H10" s="45" t="s">
+      <c r="G10" s="43"/>
+      <c r="H10" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="46"/>
-      <c r="J10" s="47"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="46"/>
       <c r="K10" s="15" t="s">
         <v>20</v>
       </c>
@@ -2312,21 +2309,21 @@
       <c r="A11" s="4">
         <v>1</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="48" t="s">
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="48"/>
-      <c r="H11" s="45" t="s">
+      <c r="G11" s="47"/>
+      <c r="H11" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="I11" s="46"/>
-      <c r="J11" s="47"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="46"/>
       <c r="K11" s="15"/>
       <c r="L11" s="5"/>
     </row>
@@ -2334,21 +2331,21 @@
       <c r="A12" s="4">
         <v>2</v>
       </c>
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="48" t="s">
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="48"/>
-      <c r="H12" s="45" t="s">
+      <c r="G12" s="47"/>
+      <c r="H12" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="I12" s="46"/>
-      <c r="J12" s="47"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="46"/>
       <c r="K12" s="15"/>
       <c r="L12" s="5"/>
     </row>
@@ -2356,21 +2353,21 @@
       <c r="A13" s="4">
         <v>3</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="48" t="s">
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="48"/>
-      <c r="H13" s="45" t="s">
+      <c r="G13" s="47"/>
+      <c r="H13" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="I13" s="46"/>
-      <c r="J13" s="47"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="46"/>
       <c r="K13" s="15"/>
       <c r="L13" s="5"/>
       <c r="M13"/>
@@ -2379,21 +2376,21 @@
       <c r="A14" s="4">
         <v>4</v>
       </c>
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="48" t="s">
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="48"/>
-      <c r="H14" s="45" t="s">
+      <c r="G14" s="47"/>
+      <c r="H14" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="I14" s="46"/>
-      <c r="J14" s="47"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="46"/>
       <c r="K14" s="15"/>
       <c r="L14" s="5"/>
       <c r="M14"/>
@@ -2402,19 +2399,19 @@
       <c r="A15" s="4">
         <v>5</v>
       </c>
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="48" t="s">
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="48"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="46"/>
       <c r="K15" s="15">
         <v>0.67</v>
       </c>
@@ -2425,19 +2422,19 @@
       <c r="A16" s="4">
         <v>6</v>
       </c>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="48" t="s">
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="48"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="46"/>
       <c r="K16" s="15">
         <v>320.5</v>
       </c>
@@ -2448,19 +2445,19 @@
       <c r="A17" s="4">
         <v>7</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="48" t="s">
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="48"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="46"/>
       <c r="K17" s="15">
         <v>32.299999999999997</v>
       </c>
@@ -2471,19 +2468,19 @@
       <c r="A18" s="4">
         <v>8</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="48" t="s">
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="48"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="46"/>
       <c r="K18" s="15">
         <v>0.91</v>
       </c>
@@ -2494,19 +2491,19 @@
       <c r="A19" s="4">
         <v>9</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="48" t="s">
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="48"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="46"/>
       <c r="K19" s="15">
         <v>0.93</v>
       </c>
@@ -2519,12 +2516,12 @@
       <c r="M20"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
       <c r="F21" s="1">
         <v>1000</v>
       </c>
@@ -2636,62 +2633,62 @@
       <c r="L30"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="54" t="str">
+      <c r="A31" s="53" t="str">
         <f>"Выводы: по сценариям Р90, Р50, Р10 получилось, что с вероятностью 90% начальные геологические запасы газа составят "&amp;C25&amp;" млрд м3, с вероятностью 50% - "&amp;C27&amp;" млрд м3,  с вероятностью 10% - "&amp;C29&amp;" млрд м3"</f>
         <v>Выводы: по сценариям Р90, Р50, Р10 получилось, что с вероятностью 90% начальные геологические запасы газа составят 6655,5 млрд м3, с вероятностью 50% - 8530,8 млрд м3,  с вероятностью 10% - 10406,1 млрд м3</v>
       </c>
-      <c r="B31" s="54"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="54"/>
-      <c r="H31" s="54"/>
-      <c r="I31" s="54"/>
-      <c r="J31" s="54"/>
-      <c r="K31" s="54"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="53"/>
+      <c r="K31" s="53"/>
       <c r="L31"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="54"/>
-      <c r="B32" s="54"/>
-      <c r="C32" s="54"/>
-      <c r="D32" s="54"/>
-      <c r="E32" s="54"/>
-      <c r="F32" s="54"/>
-      <c r="G32" s="54"/>
-      <c r="H32" s="54"/>
-      <c r="I32" s="54"/>
-      <c r="J32" s="54"/>
-      <c r="K32" s="54"/>
+      <c r="A32" s="53"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="53"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="53"/>
+      <c r="I32" s="53"/>
+      <c r="J32" s="53"/>
+      <c r="K32" s="53"/>
       <c r="L32"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="54"/>
-      <c r="B33" s="54"/>
-      <c r="C33" s="54"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="54"/>
-      <c r="H33" s="54"/>
-      <c r="I33" s="54"/>
-      <c r="J33" s="54"/>
-      <c r="K33" s="54"/>
+      <c r="A33" s="53"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="53"/>
+      <c r="K33" s="53"/>
       <c r="L33"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="54"/>
-      <c r="B34" s="54"/>
-      <c r="C34" s="54"/>
-      <c r="D34" s="54"/>
-      <c r="E34" s="54"/>
-      <c r="F34" s="54"/>
-      <c r="G34" s="54"/>
-      <c r="H34" s="54"/>
-      <c r="I34" s="54"/>
-      <c r="J34" s="54"/>
-      <c r="K34" s="54"/>
+      <c r="A34" s="53"/>
+      <c r="B34" s="53"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="53"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="53"/>
+      <c r="K34" s="53"/>
       <c r="L34"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2872,740 +2869,740 @@
       <c r="L53"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="44"/>
-      <c r="B54" s="44"/>
-      <c r="C54" s="44"/>
-      <c r="D54" s="44"/>
-      <c r="E54" s="44"/>
-      <c r="F54" s="44"/>
-      <c r="G54" s="44"/>
-      <c r="H54" s="44"/>
-      <c r="I54" s="44"/>
-      <c r="J54" s="44"/>
-      <c r="K54" s="44"/>
+      <c r="A54" s="43"/>
+      <c r="B54" s="43"/>
+      <c r="C54" s="43"/>
+      <c r="D54" s="43"/>
+      <c r="E54" s="43"/>
+      <c r="F54" s="43"/>
+      <c r="G54" s="43"/>
+      <c r="H54" s="43"/>
+      <c r="I54" s="43"/>
+      <c r="J54" s="43"/>
+      <c r="K54" s="43"/>
       <c r="L54"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="44"/>
-      <c r="B55" s="44"/>
-      <c r="C55" s="44"/>
-      <c r="D55" s="44"/>
-      <c r="E55" s="44"/>
-      <c r="F55" s="44"/>
-      <c r="G55" s="44"/>
-      <c r="H55" s="44"/>
-      <c r="I55" s="44"/>
-      <c r="J55" s="44"/>
-      <c r="K55" s="44"/>
+      <c r="A55" s="43"/>
+      <c r="B55" s="43"/>
+      <c r="C55" s="43"/>
+      <c r="D55" s="43"/>
+      <c r="E55" s="43"/>
+      <c r="F55" s="43"/>
+      <c r="G55" s="43"/>
+      <c r="H55" s="43"/>
+      <c r="I55" s="43"/>
+      <c r="J55" s="43"/>
+      <c r="K55" s="43"/>
       <c r="L55"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" s="44"/>
-      <c r="B56" s="44"/>
-      <c r="C56" s="44"/>
-      <c r="D56" s="44"/>
-      <c r="E56" s="44"/>
-      <c r="F56" s="44"/>
-      <c r="G56" s="44"/>
-      <c r="H56" s="44"/>
-      <c r="I56" s="44"/>
-      <c r="J56" s="44"/>
-      <c r="K56" s="44"/>
+      <c r="A56" s="43"/>
+      <c r="B56" s="43"/>
+      <c r="C56" s="43"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="43"/>
+      <c r="F56" s="43"/>
+      <c r="G56" s="43"/>
+      <c r="H56" s="43"/>
+      <c r="I56" s="43"/>
+      <c r="J56" s="43"/>
+      <c r="K56" s="43"/>
       <c r="L56"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="44"/>
-      <c r="B57" s="44"/>
-      <c r="C57" s="44"/>
-      <c r="D57" s="44"/>
-      <c r="E57" s="44"/>
-      <c r="F57" s="44"/>
-      <c r="G57" s="44"/>
-      <c r="H57" s="44"/>
-      <c r="I57" s="44"/>
-      <c r="J57" s="44"/>
-      <c r="K57" s="44"/>
+      <c r="A57" s="43"/>
+      <c r="B57" s="43"/>
+      <c r="C57" s="43"/>
+      <c r="D57" s="43"/>
+      <c r="E57" s="43"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="43"/>
+      <c r="H57" s="43"/>
+      <c r="I57" s="43"/>
+      <c r="J57" s="43"/>
+      <c r="K57" s="43"/>
       <c r="L57"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="44"/>
-      <c r="B58" s="44"/>
-      <c r="C58" s="44"/>
-      <c r="D58" s="44"/>
-      <c r="E58" s="44"/>
-      <c r="F58" s="44"/>
-      <c r="G58" s="44"/>
-      <c r="H58" s="44"/>
-      <c r="I58" s="44"/>
-      <c r="J58" s="44"/>
-      <c r="K58" s="44"/>
+      <c r="A58" s="43"/>
+      <c r="B58" s="43"/>
+      <c r="C58" s="43"/>
+      <c r="D58" s="43"/>
+      <c r="E58" s="43"/>
+      <c r="F58" s="43"/>
+      <c r="G58" s="43"/>
+      <c r="H58" s="43"/>
+      <c r="I58" s="43"/>
+      <c r="J58" s="43"/>
+      <c r="K58" s="43"/>
       <c r="L58"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="44"/>
-      <c r="B59" s="44"/>
-      <c r="C59" s="44"/>
-      <c r="D59" s="44"/>
-      <c r="E59" s="44"/>
-      <c r="F59" s="44"/>
-      <c r="G59" s="44"/>
-      <c r="H59" s="44"/>
-      <c r="I59" s="44"/>
-      <c r="J59" s="44"/>
-      <c r="K59" s="44"/>
+      <c r="A59" s="43"/>
+      <c r="B59" s="43"/>
+      <c r="C59" s="43"/>
+      <c r="D59" s="43"/>
+      <c r="E59" s="43"/>
+      <c r="F59" s="43"/>
+      <c r="G59" s="43"/>
+      <c r="H59" s="43"/>
+      <c r="I59" s="43"/>
+      <c r="J59" s="43"/>
+      <c r="K59" s="43"/>
       <c r="L59"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="44"/>
-      <c r="B60" s="44"/>
-      <c r="C60" s="44"/>
-      <c r="D60" s="44"/>
-      <c r="E60" s="44"/>
-      <c r="F60" s="44"/>
-      <c r="G60" s="44"/>
-      <c r="H60" s="44"/>
-      <c r="I60" s="44"/>
-      <c r="J60" s="44"/>
-      <c r="K60" s="44"/>
+      <c r="A60" s="43"/>
+      <c r="B60" s="43"/>
+      <c r="C60" s="43"/>
+      <c r="D60" s="43"/>
+      <c r="E60" s="43"/>
+      <c r="F60" s="43"/>
+      <c r="G60" s="43"/>
+      <c r="H60" s="43"/>
+      <c r="I60" s="43"/>
+      <c r="J60" s="43"/>
+      <c r="K60" s="43"/>
       <c r="L60"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61" s="44"/>
-      <c r="B61" s="44"/>
-      <c r="C61" s="44"/>
-      <c r="D61" s="44"/>
-      <c r="E61" s="44"/>
-      <c r="F61" s="44"/>
-      <c r="G61" s="44"/>
-      <c r="H61" s="44"/>
-      <c r="I61" s="44"/>
-      <c r="J61" s="44"/>
-      <c r="K61" s="44"/>
+      <c r="A61" s="43"/>
+      <c r="B61" s="43"/>
+      <c r="C61" s="43"/>
+      <c r="D61" s="43"/>
+      <c r="E61" s="43"/>
+      <c r="F61" s="43"/>
+      <c r="G61" s="43"/>
+      <c r="H61" s="43"/>
+      <c r="I61" s="43"/>
+      <c r="J61" s="43"/>
+      <c r="K61" s="43"/>
       <c r="L61"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A62" s="44"/>
-      <c r="B62" s="44"/>
-      <c r="C62" s="44"/>
-      <c r="D62" s="44"/>
-      <c r="E62" s="44"/>
-      <c r="F62" s="44"/>
-      <c r="G62" s="44"/>
-      <c r="H62" s="44"/>
-      <c r="I62" s="44"/>
-      <c r="J62" s="44"/>
-      <c r="K62" s="44"/>
+      <c r="A62" s="43"/>
+      <c r="B62" s="43"/>
+      <c r="C62" s="43"/>
+      <c r="D62" s="43"/>
+      <c r="E62" s="43"/>
+      <c r="F62" s="43"/>
+      <c r="G62" s="43"/>
+      <c r="H62" s="43"/>
+      <c r="I62" s="43"/>
+      <c r="J62" s="43"/>
+      <c r="K62" s="43"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="44"/>
-      <c r="B63" s="44"/>
-      <c r="C63" s="44"/>
-      <c r="D63" s="44"/>
-      <c r="E63" s="44"/>
-      <c r="F63" s="44"/>
-      <c r="G63" s="44"/>
-      <c r="H63" s="44"/>
-      <c r="I63" s="44"/>
-      <c r="J63" s="44"/>
-      <c r="K63" s="44"/>
+      <c r="A63" s="43"/>
+      <c r="B63" s="43"/>
+      <c r="C63" s="43"/>
+      <c r="D63" s="43"/>
+      <c r="E63" s="43"/>
+      <c r="F63" s="43"/>
+      <c r="G63" s="43"/>
+      <c r="H63" s="43"/>
+      <c r="I63" s="43"/>
+      <c r="J63" s="43"/>
+      <c r="K63" s="43"/>
       <c r="L63"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A64" s="44"/>
-      <c r="B64" s="44"/>
-      <c r="C64" s="44"/>
-      <c r="D64" s="44"/>
-      <c r="E64" s="44"/>
-      <c r="F64" s="44"/>
-      <c r="G64" s="44"/>
-      <c r="H64" s="44"/>
-      <c r="I64" s="44"/>
-      <c r="J64" s="44"/>
-      <c r="K64" s="44"/>
+      <c r="A64" s="43"/>
+      <c r="B64" s="43"/>
+      <c r="C64" s="43"/>
+      <c r="D64" s="43"/>
+      <c r="E64" s="43"/>
+      <c r="F64" s="43"/>
+      <c r="G64" s="43"/>
+      <c r="H64" s="43"/>
+      <c r="I64" s="43"/>
+      <c r="J64" s="43"/>
+      <c r="K64" s="43"/>
       <c r="L64"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A65" s="44"/>
-      <c r="B65" s="44"/>
-      <c r="C65" s="44"/>
-      <c r="D65" s="44"/>
-      <c r="E65" s="44"/>
-      <c r="F65" s="44"/>
-      <c r="G65" s="44"/>
-      <c r="H65" s="44"/>
-      <c r="I65" s="44"/>
-      <c r="J65" s="44"/>
-      <c r="K65" s="44"/>
+      <c r="A65" s="43"/>
+      <c r="B65" s="43"/>
+      <c r="C65" s="43"/>
+      <c r="D65" s="43"/>
+      <c r="E65" s="43"/>
+      <c r="F65" s="43"/>
+      <c r="G65" s="43"/>
+      <c r="H65" s="43"/>
+      <c r="I65" s="43"/>
+      <c r="J65" s="43"/>
+      <c r="K65" s="43"/>
       <c r="L65"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A66" s="44"/>
-      <c r="B66" s="44"/>
-      <c r="C66" s="44"/>
-      <c r="D66" s="44"/>
-      <c r="E66" s="44"/>
-      <c r="F66" s="44"/>
-      <c r="G66" s="44"/>
-      <c r="H66" s="44"/>
-      <c r="I66" s="44"/>
-      <c r="J66" s="44"/>
-      <c r="K66" s="44"/>
+      <c r="A66" s="43"/>
+      <c r="B66" s="43"/>
+      <c r="C66" s="43"/>
+      <c r="D66" s="43"/>
+      <c r="E66" s="43"/>
+      <c r="F66" s="43"/>
+      <c r="G66" s="43"/>
+      <c r="H66" s="43"/>
+      <c r="I66" s="43"/>
+      <c r="J66" s="43"/>
+      <c r="K66" s="43"/>
       <c r="L66"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A67" s="44"/>
-      <c r="B67" s="44"/>
-      <c r="C67" s="44"/>
-      <c r="D67" s="44"/>
-      <c r="E67" s="44"/>
-      <c r="F67" s="44"/>
-      <c r="G67" s="44"/>
-      <c r="H67" s="44"/>
-      <c r="I67" s="44"/>
-      <c r="J67" s="44"/>
-      <c r="K67" s="44"/>
+      <c r="A67" s="43"/>
+      <c r="B67" s="43"/>
+      <c r="C67" s="43"/>
+      <c r="D67" s="43"/>
+      <c r="E67" s="43"/>
+      <c r="F67" s="43"/>
+      <c r="G67" s="43"/>
+      <c r="H67" s="43"/>
+      <c r="I67" s="43"/>
+      <c r="J67" s="43"/>
+      <c r="K67" s="43"/>
       <c r="L67"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A68" s="44"/>
-      <c r="B68" s="44"/>
-      <c r="C68" s="44"/>
-      <c r="D68" s="44"/>
-      <c r="E68" s="44"/>
-      <c r="F68" s="44"/>
-      <c r="G68" s="44"/>
-      <c r="H68" s="44"/>
-      <c r="I68" s="44"/>
-      <c r="J68" s="44"/>
-      <c r="K68" s="44"/>
+      <c r="A68" s="43"/>
+      <c r="B68" s="43"/>
+      <c r="C68" s="43"/>
+      <c r="D68" s="43"/>
+      <c r="E68" s="43"/>
+      <c r="F68" s="43"/>
+      <c r="G68" s="43"/>
+      <c r="H68" s="43"/>
+      <c r="I68" s="43"/>
+      <c r="J68" s="43"/>
+      <c r="K68" s="43"/>
       <c r="L68"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A69" s="44"/>
-      <c r="B69" s="44"/>
-      <c r="C69" s="44"/>
-      <c r="D69" s="44"/>
-      <c r="E69" s="44"/>
-      <c r="F69" s="44"/>
-      <c r="G69" s="44"/>
-      <c r="H69" s="44"/>
-      <c r="I69" s="44"/>
-      <c r="J69" s="44"/>
-      <c r="K69" s="44"/>
+      <c r="A69" s="43"/>
+      <c r="B69" s="43"/>
+      <c r="C69" s="43"/>
+      <c r="D69" s="43"/>
+      <c r="E69" s="43"/>
+      <c r="F69" s="43"/>
+      <c r="G69" s="43"/>
+      <c r="H69" s="43"/>
+      <c r="I69" s="43"/>
+      <c r="J69" s="43"/>
+      <c r="K69" s="43"/>
       <c r="L69"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" s="44"/>
-      <c r="B70" s="44"/>
-      <c r="C70" s="44"/>
-      <c r="D70" s="44"/>
-      <c r="E70" s="44"/>
-      <c r="F70" s="44"/>
-      <c r="G70" s="44"/>
-      <c r="H70" s="44"/>
-      <c r="I70" s="44"/>
-      <c r="J70" s="44"/>
-      <c r="K70" s="44"/>
+      <c r="A70" s="43"/>
+      <c r="B70" s="43"/>
+      <c r="C70" s="43"/>
+      <c r="D70" s="43"/>
+      <c r="E70" s="43"/>
+      <c r="F70" s="43"/>
+      <c r="G70" s="43"/>
+      <c r="H70" s="43"/>
+      <c r="I70" s="43"/>
+      <c r="J70" s="43"/>
+      <c r="K70" s="43"/>
       <c r="L70"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A71" s="44"/>
-      <c r="B71" s="44"/>
-      <c r="C71" s="44"/>
-      <c r="D71" s="44"/>
-      <c r="E71" s="44"/>
-      <c r="F71" s="44"/>
-      <c r="G71" s="44"/>
-      <c r="H71" s="44"/>
-      <c r="I71" s="44"/>
-      <c r="J71" s="44"/>
-      <c r="K71" s="44"/>
+      <c r="A71" s="43"/>
+      <c r="B71" s="43"/>
+      <c r="C71" s="43"/>
+      <c r="D71" s="43"/>
+      <c r="E71" s="43"/>
+      <c r="F71" s="43"/>
+      <c r="G71" s="43"/>
+      <c r="H71" s="43"/>
+      <c r="I71" s="43"/>
+      <c r="J71" s="43"/>
+      <c r="K71" s="43"/>
       <c r="L71"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A72" s="44"/>
-      <c r="B72" s="44"/>
-      <c r="C72" s="44"/>
-      <c r="D72" s="44"/>
-      <c r="E72" s="44"/>
-      <c r="F72" s="44"/>
-      <c r="G72" s="44"/>
-      <c r="H72" s="44"/>
-      <c r="I72" s="44"/>
-      <c r="J72" s="44"/>
-      <c r="K72" s="44"/>
+      <c r="A72" s="43"/>
+      <c r="B72" s="43"/>
+      <c r="C72" s="43"/>
+      <c r="D72" s="43"/>
+      <c r="E72" s="43"/>
+      <c r="F72" s="43"/>
+      <c r="G72" s="43"/>
+      <c r="H72" s="43"/>
+      <c r="I72" s="43"/>
+      <c r="J72" s="43"/>
+      <c r="K72" s="43"/>
       <c r="L72"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A73" s="44"/>
-      <c r="B73" s="44"/>
-      <c r="C73" s="44"/>
-      <c r="D73" s="44"/>
-      <c r="E73" s="44"/>
-      <c r="F73" s="44"/>
-      <c r="G73" s="44"/>
-      <c r="H73" s="44"/>
-      <c r="I73" s="44"/>
-      <c r="J73" s="44"/>
-      <c r="K73" s="44"/>
+      <c r="A73" s="43"/>
+      <c r="B73" s="43"/>
+      <c r="C73" s="43"/>
+      <c r="D73" s="43"/>
+      <c r="E73" s="43"/>
+      <c r="F73" s="43"/>
+      <c r="G73" s="43"/>
+      <c r="H73" s="43"/>
+      <c r="I73" s="43"/>
+      <c r="J73" s="43"/>
+      <c r="K73" s="43"/>
       <c r="L73"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A74" s="44"/>
-      <c r="B74" s="44"/>
-      <c r="C74" s="44"/>
-      <c r="D74" s="44"/>
-      <c r="E74" s="44"/>
-      <c r="F74" s="44"/>
-      <c r="G74" s="44"/>
-      <c r="H74" s="44"/>
-      <c r="I74" s="44"/>
-      <c r="J74" s="44"/>
-      <c r="K74" s="44"/>
+      <c r="A74" s="43"/>
+      <c r="B74" s="43"/>
+      <c r="C74" s="43"/>
+      <c r="D74" s="43"/>
+      <c r="E74" s="43"/>
+      <c r="F74" s="43"/>
+      <c r="G74" s="43"/>
+      <c r="H74" s="43"/>
+      <c r="I74" s="43"/>
+      <c r="J74" s="43"/>
+      <c r="K74" s="43"/>
       <c r="L74"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A75" s="44"/>
-      <c r="B75" s="44"/>
-      <c r="C75" s="44"/>
-      <c r="D75" s="44"/>
-      <c r="E75" s="44"/>
-      <c r="F75" s="44"/>
-      <c r="G75" s="44"/>
-      <c r="H75" s="44"/>
-      <c r="I75" s="44"/>
-      <c r="J75" s="44"/>
-      <c r="K75" s="44"/>
+      <c r="A75" s="43"/>
+      <c r="B75" s="43"/>
+      <c r="C75" s="43"/>
+      <c r="D75" s="43"/>
+      <c r="E75" s="43"/>
+      <c r="F75" s="43"/>
+      <c r="G75" s="43"/>
+      <c r="H75" s="43"/>
+      <c r="I75" s="43"/>
+      <c r="J75" s="43"/>
+      <c r="K75" s="43"/>
       <c r="L75"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A76" s="44"/>
-      <c r="B76" s="44"/>
-      <c r="C76" s="44"/>
-      <c r="D76" s="44"/>
-      <c r="E76" s="44"/>
-      <c r="F76" s="44"/>
-      <c r="G76" s="44"/>
-      <c r="H76" s="44"/>
-      <c r="I76" s="44"/>
-      <c r="J76" s="44"/>
-      <c r="K76" s="44"/>
+      <c r="A76" s="43"/>
+      <c r="B76" s="43"/>
+      <c r="C76" s="43"/>
+      <c r="D76" s="43"/>
+      <c r="E76" s="43"/>
+      <c r="F76" s="43"/>
+      <c r="G76" s="43"/>
+      <c r="H76" s="43"/>
+      <c r="I76" s="43"/>
+      <c r="J76" s="43"/>
+      <c r="K76" s="43"/>
       <c r="L76"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A77" s="44"/>
-      <c r="B77" s="44"/>
-      <c r="C77" s="44"/>
-      <c r="D77" s="44"/>
-      <c r="E77" s="44"/>
-      <c r="F77" s="44"/>
-      <c r="G77" s="44"/>
-      <c r="H77" s="44"/>
-      <c r="I77" s="44"/>
-      <c r="J77" s="44"/>
-      <c r="K77" s="44"/>
+      <c r="A77" s="43"/>
+      <c r="B77" s="43"/>
+      <c r="C77" s="43"/>
+      <c r="D77" s="43"/>
+      <c r="E77" s="43"/>
+      <c r="F77" s="43"/>
+      <c r="G77" s="43"/>
+      <c r="H77" s="43"/>
+      <c r="I77" s="43"/>
+      <c r="J77" s="43"/>
+      <c r="K77" s="43"/>
       <c r="L77"/>
     </row>
     <row r="78" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="44"/>
-      <c r="B78" s="44"/>
-      <c r="C78" s="44"/>
-      <c r="D78" s="44"/>
-      <c r="E78" s="44"/>
-      <c r="F78" s="44"/>
-      <c r="G78" s="44"/>
-      <c r="H78" s="44"/>
-      <c r="I78" s="44"/>
-      <c r="J78" s="44"/>
-      <c r="K78" s="44"/>
+      <c r="A78" s="43"/>
+      <c r="B78" s="43"/>
+      <c r="C78" s="43"/>
+      <c r="D78" s="43"/>
+      <c r="E78" s="43"/>
+      <c r="F78" s="43"/>
+      <c r="G78" s="43"/>
+      <c r="H78" s="43"/>
+      <c r="I78" s="43"/>
+      <c r="J78" s="43"/>
+      <c r="K78" s="43"/>
       <c r="L78"/>
     </row>
     <row r="79" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="66" t="s">
+      <c r="A79" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="B79" s="66"/>
-      <c r="C79" s="66"/>
-      <c r="D79" s="66"/>
-      <c r="E79" s="66"/>
-      <c r="F79" s="66"/>
-      <c r="G79" s="66"/>
-      <c r="H79" s="66"/>
-      <c r="I79" s="66"/>
-      <c r="J79" s="66"/>
-      <c r="K79" s="66"/>
+      <c r="B79" s="55"/>
+      <c r="C79" s="55"/>
+      <c r="D79" s="55"/>
+      <c r="E79" s="55"/>
+      <c r="F79" s="55"/>
+      <c r="G79" s="55"/>
+      <c r="H79" s="55"/>
+      <c r="I79" s="55"/>
+      <c r="J79" s="55"/>
+      <c r="K79" s="55"/>
       <c r="L79"/>
     </row>
     <row r="80" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="66"/>
-      <c r="B80" s="66"/>
-      <c r="C80" s="66"/>
-      <c r="D80" s="66"/>
-      <c r="E80" s="66"/>
-      <c r="F80" s="66"/>
-      <c r="G80" s="66"/>
-      <c r="H80" s="66"/>
-      <c r="I80" s="66"/>
-      <c r="J80" s="66"/>
-      <c r="K80" s="66"/>
+      <c r="A80" s="55"/>
+      <c r="B80" s="55"/>
+      <c r="C80" s="55"/>
+      <c r="D80" s="55"/>
+      <c r="E80" s="55"/>
+      <c r="F80" s="55"/>
+      <c r="G80" s="55"/>
+      <c r="H80" s="55"/>
+      <c r="I80" s="55"/>
+      <c r="J80" s="55"/>
+      <c r="K80" s="55"/>
       <c r="L80"/>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A81" s="66"/>
-      <c r="B81" s="66"/>
-      <c r="C81" s="66"/>
-      <c r="D81" s="66"/>
-      <c r="E81" s="66"/>
-      <c r="F81" s="66"/>
-      <c r="G81" s="66"/>
-      <c r="H81" s="66"/>
-      <c r="I81" s="66"/>
-      <c r="J81" s="66"/>
-      <c r="K81" s="66"/>
+      <c r="A81" s="55"/>
+      <c r="B81" s="55"/>
+      <c r="C81" s="55"/>
+      <c r="D81" s="55"/>
+      <c r="E81" s="55"/>
+      <c r="F81" s="55"/>
+      <c r="G81" s="55"/>
+      <c r="H81" s="55"/>
+      <c r="I81" s="55"/>
+      <c r="J81" s="55"/>
+      <c r="K81" s="55"/>
       <c r="L81"/>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A82" s="44"/>
-      <c r="B82" s="44"/>
-      <c r="C82" s="44"/>
-      <c r="D82" s="44"/>
-      <c r="E82" s="44"/>
-      <c r="F82" s="44"/>
-      <c r="G82" s="44"/>
-      <c r="H82" s="44"/>
-      <c r="I82" s="44"/>
-      <c r="J82" s="44"/>
-      <c r="K82" s="44"/>
+      <c r="A82" s="43"/>
+      <c r="B82" s="43"/>
+      <c r="C82" s="43"/>
+      <c r="D82" s="43"/>
+      <c r="E82" s="43"/>
+      <c r="F82" s="43"/>
+      <c r="G82" s="43"/>
+      <c r="H82" s="43"/>
+      <c r="I82" s="43"/>
+      <c r="J82" s="43"/>
+      <c r="K82" s="43"/>
       <c r="L82"/>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A83" s="44"/>
-      <c r="B83" s="44"/>
-      <c r="C83" s="44"/>
-      <c r="D83" s="44"/>
-      <c r="E83" s="44"/>
-      <c r="F83" s="44"/>
-      <c r="G83" s="44"/>
-      <c r="H83" s="44"/>
-      <c r="I83" s="44"/>
-      <c r="J83" s="44"/>
-      <c r="K83" s="44"/>
+      <c r="A83" s="43"/>
+      <c r="B83" s="43"/>
+      <c r="C83" s="43"/>
+      <c r="D83" s="43"/>
+      <c r="E83" s="43"/>
+      <c r="F83" s="43"/>
+      <c r="G83" s="43"/>
+      <c r="H83" s="43"/>
+      <c r="I83" s="43"/>
+      <c r="J83" s="43"/>
+      <c r="K83" s="43"/>
       <c r="L83"/>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A84" s="44"/>
-      <c r="B84" s="44"/>
-      <c r="C84" s="44"/>
-      <c r="D84" s="44"/>
-      <c r="E84" s="44"/>
-      <c r="F84" s="44"/>
-      <c r="G84" s="44"/>
-      <c r="H84" s="44"/>
-      <c r="I84" s="44"/>
-      <c r="J84" s="44"/>
-      <c r="K84" s="44"/>
+      <c r="A84" s="43"/>
+      <c r="B84" s="43"/>
+      <c r="C84" s="43"/>
+      <c r="D84" s="43"/>
+      <c r="E84" s="43"/>
+      <c r="F84" s="43"/>
+      <c r="G84" s="43"/>
+      <c r="H84" s="43"/>
+      <c r="I84" s="43"/>
+      <c r="J84" s="43"/>
+      <c r="K84" s="43"/>
       <c r="L84"/>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A85" s="44"/>
-      <c r="B85" s="44"/>
-      <c r="C85" s="44"/>
-      <c r="D85" s="44"/>
-      <c r="E85" s="44"/>
-      <c r="F85" s="44"/>
-      <c r="G85" s="44"/>
-      <c r="H85" s="44"/>
-      <c r="I85" s="44"/>
-      <c r="J85" s="44"/>
-      <c r="K85" s="44"/>
+      <c r="A85" s="43"/>
+      <c r="B85" s="43"/>
+      <c r="C85" s="43"/>
+      <c r="D85" s="43"/>
+      <c r="E85" s="43"/>
+      <c r="F85" s="43"/>
+      <c r="G85" s="43"/>
+      <c r="H85" s="43"/>
+      <c r="I85" s="43"/>
+      <c r="J85" s="43"/>
+      <c r="K85" s="43"/>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A86" s="44"/>
-      <c r="B86" s="44"/>
-      <c r="C86" s="44"/>
-      <c r="D86" s="44"/>
-      <c r="E86" s="44"/>
-      <c r="F86" s="44"/>
-      <c r="G86" s="44"/>
-      <c r="H86" s="44"/>
-      <c r="I86" s="44"/>
-      <c r="J86" s="44"/>
-      <c r="K86" s="44"/>
+      <c r="A86" s="43"/>
+      <c r="B86" s="43"/>
+      <c r="C86" s="43"/>
+      <c r="D86" s="43"/>
+      <c r="E86" s="43"/>
+      <c r="F86" s="43"/>
+      <c r="G86" s="43"/>
+      <c r="H86" s="43"/>
+      <c r="I86" s="43"/>
+      <c r="J86" s="43"/>
+      <c r="K86" s="43"/>
       <c r="L86"/>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A87" s="44"/>
-      <c r="B87" s="44"/>
-      <c r="C87" s="44"/>
-      <c r="D87" s="44"/>
-      <c r="E87" s="44"/>
-      <c r="F87" s="44"/>
-      <c r="G87" s="44"/>
-      <c r="H87" s="44"/>
-      <c r="I87" s="44"/>
-      <c r="J87" s="44"/>
-      <c r="K87" s="44"/>
+      <c r="A87" s="43"/>
+      <c r="B87" s="43"/>
+      <c r="C87" s="43"/>
+      <c r="D87" s="43"/>
+      <c r="E87" s="43"/>
+      <c r="F87" s="43"/>
+      <c r="G87" s="43"/>
+      <c r="H87" s="43"/>
+      <c r="I87" s="43"/>
+      <c r="J87" s="43"/>
+      <c r="K87" s="43"/>
       <c r="L87"/>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A88" s="44"/>
-      <c r="B88" s="44"/>
-      <c r="C88" s="44"/>
-      <c r="D88" s="44"/>
-      <c r="E88" s="44"/>
-      <c r="F88" s="44"/>
-      <c r="G88" s="44"/>
-      <c r="H88" s="44"/>
-      <c r="I88" s="44"/>
-      <c r="J88" s="44"/>
-      <c r="K88" s="44"/>
+      <c r="A88" s="43"/>
+      <c r="B88" s="43"/>
+      <c r="C88" s="43"/>
+      <c r="D88" s="43"/>
+      <c r="E88" s="43"/>
+      <c r="F88" s="43"/>
+      <c r="G88" s="43"/>
+      <c r="H88" s="43"/>
+      <c r="I88" s="43"/>
+      <c r="J88" s="43"/>
+      <c r="K88" s="43"/>
       <c r="L88"/>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A89" s="44"/>
-      <c r="B89" s="44"/>
-      <c r="C89" s="44"/>
-      <c r="D89" s="44"/>
-      <c r="E89" s="44"/>
-      <c r="F89" s="44"/>
-      <c r="G89" s="44"/>
-      <c r="H89" s="44"/>
-      <c r="I89" s="44"/>
-      <c r="J89" s="44"/>
-      <c r="K89" s="44"/>
+      <c r="A89" s="43"/>
+      <c r="B89" s="43"/>
+      <c r="C89" s="43"/>
+      <c r="D89" s="43"/>
+      <c r="E89" s="43"/>
+      <c r="F89" s="43"/>
+      <c r="G89" s="43"/>
+      <c r="H89" s="43"/>
+      <c r="I89" s="43"/>
+      <c r="J89" s="43"/>
+      <c r="K89" s="43"/>
       <c r="L89"/>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A90" s="44"/>
-      <c r="B90" s="44"/>
-      <c r="C90" s="44"/>
-      <c r="D90" s="44"/>
-      <c r="E90" s="44"/>
-      <c r="F90" s="44"/>
-      <c r="G90" s="44"/>
-      <c r="H90" s="44"/>
-      <c r="I90" s="44"/>
-      <c r="J90" s="44"/>
-      <c r="K90" s="44"/>
+      <c r="A90" s="43"/>
+      <c r="B90" s="43"/>
+      <c r="C90" s="43"/>
+      <c r="D90" s="43"/>
+      <c r="E90" s="43"/>
+      <c r="F90" s="43"/>
+      <c r="G90" s="43"/>
+      <c r="H90" s="43"/>
+      <c r="I90" s="43"/>
+      <c r="J90" s="43"/>
+      <c r="K90" s="43"/>
       <c r="L90"/>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A91" s="44"/>
-      <c r="B91" s="44"/>
-      <c r="C91" s="44"/>
-      <c r="D91" s="44"/>
-      <c r="E91" s="44"/>
-      <c r="F91" s="44"/>
-      <c r="G91" s="44"/>
-      <c r="H91" s="44"/>
-      <c r="I91" s="44"/>
-      <c r="J91" s="44"/>
-      <c r="K91" s="44"/>
+      <c r="A91" s="43"/>
+      <c r="B91" s="43"/>
+      <c r="C91" s="43"/>
+      <c r="D91" s="43"/>
+      <c r="E91" s="43"/>
+      <c r="F91" s="43"/>
+      <c r="G91" s="43"/>
+      <c r="H91" s="43"/>
+      <c r="I91" s="43"/>
+      <c r="J91" s="43"/>
+      <c r="K91" s="43"/>
       <c r="L91"/>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A92" s="44"/>
-      <c r="B92" s="44"/>
-      <c r="C92" s="44"/>
-      <c r="D92" s="44"/>
-      <c r="E92" s="44"/>
-      <c r="F92" s="44"/>
-      <c r="G92" s="44"/>
-      <c r="H92" s="44"/>
-      <c r="I92" s="44"/>
-      <c r="J92" s="44"/>
-      <c r="K92" s="44"/>
+      <c r="A92" s="43"/>
+      <c r="B92" s="43"/>
+      <c r="C92" s="43"/>
+      <c r="D92" s="43"/>
+      <c r="E92" s="43"/>
+      <c r="F92" s="43"/>
+      <c r="G92" s="43"/>
+      <c r="H92" s="43"/>
+      <c r="I92" s="43"/>
+      <c r="J92" s="43"/>
+      <c r="K92" s="43"/>
       <c r="L92"/>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A93" s="44"/>
-      <c r="B93" s="44"/>
-      <c r="C93" s="44"/>
-      <c r="D93" s="44"/>
-      <c r="E93" s="44"/>
-      <c r="F93" s="44"/>
-      <c r="G93" s="44"/>
-      <c r="H93" s="44"/>
-      <c r="I93" s="44"/>
-      <c r="J93" s="44"/>
-      <c r="K93" s="44"/>
+      <c r="A93" s="43"/>
+      <c r="B93" s="43"/>
+      <c r="C93" s="43"/>
+      <c r="D93" s="43"/>
+      <c r="E93" s="43"/>
+      <c r="F93" s="43"/>
+      <c r="G93" s="43"/>
+      <c r="H93" s="43"/>
+      <c r="I93" s="43"/>
+      <c r="J93" s="43"/>
+      <c r="K93" s="43"/>
       <c r="L93"/>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A94" s="44"/>
-      <c r="B94" s="44"/>
-      <c r="C94" s="44"/>
-      <c r="D94" s="44"/>
-      <c r="E94" s="44"/>
-      <c r="F94" s="44"/>
-      <c r="G94" s="44"/>
-      <c r="H94" s="44"/>
-      <c r="I94" s="44"/>
-      <c r="J94" s="44"/>
-      <c r="K94" s="44"/>
+      <c r="A94" s="43"/>
+      <c r="B94" s="43"/>
+      <c r="C94" s="43"/>
+      <c r="D94" s="43"/>
+      <c r="E94" s="43"/>
+      <c r="F94" s="43"/>
+      <c r="G94" s="43"/>
+      <c r="H94" s="43"/>
+      <c r="I94" s="43"/>
+      <c r="J94" s="43"/>
+      <c r="K94" s="43"/>
       <c r="L94"/>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A95" s="44"/>
-      <c r="B95" s="44"/>
-      <c r="C95" s="44"/>
-      <c r="D95" s="44"/>
-      <c r="E95" s="44"/>
-      <c r="F95" s="44"/>
-      <c r="G95" s="44"/>
-      <c r="H95" s="44"/>
-      <c r="I95" s="44"/>
-      <c r="J95" s="44"/>
-      <c r="K95" s="44"/>
+      <c r="A95" s="43"/>
+      <c r="B95" s="43"/>
+      <c r="C95" s="43"/>
+      <c r="D95" s="43"/>
+      <c r="E95" s="43"/>
+      <c r="F95" s="43"/>
+      <c r="G95" s="43"/>
+      <c r="H95" s="43"/>
+      <c r="I95" s="43"/>
+      <c r="J95" s="43"/>
+      <c r="K95" s="43"/>
       <c r="L95"/>
     </row>
     <row r="96" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="44"/>
-      <c r="B96" s="44"/>
-      <c r="C96" s="44"/>
-      <c r="D96" s="44"/>
-      <c r="E96" s="44"/>
-      <c r="F96" s="44"/>
-      <c r="G96" s="44"/>
-      <c r="H96" s="44"/>
-      <c r="I96" s="44"/>
-      <c r="J96" s="44"/>
-      <c r="K96" s="44"/>
+      <c r="A96" s="43"/>
+      <c r="B96" s="43"/>
+      <c r="C96" s="43"/>
+      <c r="D96" s="43"/>
+      <c r="E96" s="43"/>
+      <c r="F96" s="43"/>
+      <c r="G96" s="43"/>
+      <c r="H96" s="43"/>
+      <c r="I96" s="43"/>
+      <c r="J96" s="43"/>
+      <c r="K96" s="43"/>
       <c r="L96" s="11"/>
     </row>
     <row r="97" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="44"/>
-      <c r="B97" s="44"/>
-      <c r="C97" s="44"/>
-      <c r="D97" s="44"/>
-      <c r="E97" s="44"/>
-      <c r="F97" s="44"/>
-      <c r="G97" s="44"/>
-      <c r="H97" s="44"/>
-      <c r="I97" s="44"/>
-      <c r="J97" s="44"/>
-      <c r="K97" s="44"/>
+      <c r="A97" s="43"/>
+      <c r="B97" s="43"/>
+      <c r="C97" s="43"/>
+      <c r="D97" s="43"/>
+      <c r="E97" s="43"/>
+      <c r="F97" s="43"/>
+      <c r="G97" s="43"/>
+      <c r="H97" s="43"/>
+      <c r="I97" s="43"/>
+      <c r="J97" s="43"/>
+      <c r="K97" s="43"/>
       <c r="L97" s="11"/>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A98" s="44"/>
-      <c r="B98" s="44"/>
-      <c r="C98" s="44"/>
-      <c r="D98" s="44"/>
-      <c r="E98" s="44"/>
-      <c r="F98" s="44"/>
-      <c r="G98" s="44"/>
-      <c r="H98" s="44"/>
-      <c r="I98" s="44"/>
-      <c r="J98" s="44"/>
-      <c r="K98" s="44"/>
+      <c r="A98" s="43"/>
+      <c r="B98" s="43"/>
+      <c r="C98" s="43"/>
+      <c r="D98" s="43"/>
+      <c r="E98" s="43"/>
+      <c r="F98" s="43"/>
+      <c r="G98" s="43"/>
+      <c r="H98" s="43"/>
+      <c r="I98" s="43"/>
+      <c r="J98" s="43"/>
+      <c r="K98" s="43"/>
     </row>
     <row r="99" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A99" s="44"/>
-      <c r="B99" s="44"/>
-      <c r="C99" s="44"/>
-      <c r="D99" s="44"/>
-      <c r="E99" s="44"/>
-      <c r="F99" s="44"/>
-      <c r="G99" s="44"/>
-      <c r="H99" s="44"/>
-      <c r="I99" s="44"/>
-      <c r="J99" s="44"/>
-      <c r="K99" s="44"/>
+      <c r="A99" s="43"/>
+      <c r="B99" s="43"/>
+      <c r="C99" s="43"/>
+      <c r="D99" s="43"/>
+      <c r="E99" s="43"/>
+      <c r="F99" s="43"/>
+      <c r="G99" s="43"/>
+      <c r="H99" s="43"/>
+      <c r="I99" s="43"/>
+      <c r="J99" s="43"/>
+      <c r="K99" s="43"/>
       <c r="L99" s="17"/>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A100" s="44"/>
-      <c r="B100" s="44"/>
-      <c r="C100" s="44"/>
-      <c r="D100" s="44"/>
-      <c r="E100" s="44"/>
-      <c r="F100" s="44"/>
-      <c r="G100" s="44"/>
-      <c r="H100" s="44"/>
-      <c r="I100" s="44"/>
-      <c r="J100" s="44"/>
-      <c r="K100" s="44"/>
+      <c r="A100" s="43"/>
+      <c r="B100" s="43"/>
+      <c r="C100" s="43"/>
+      <c r="D100" s="43"/>
+      <c r="E100" s="43"/>
+      <c r="F100" s="43"/>
+      <c r="G100" s="43"/>
+      <c r="H100" s="43"/>
+      <c r="I100" s="43"/>
+      <c r="J100" s="43"/>
+      <c r="K100" s="43"/>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A101" s="44"/>
-      <c r="B101" s="44"/>
-      <c r="C101" s="44"/>
-      <c r="D101" s="44"/>
-      <c r="E101" s="44"/>
-      <c r="F101" s="44"/>
-      <c r="G101" s="44"/>
-      <c r="H101" s="44"/>
-      <c r="I101" s="44"/>
-      <c r="J101" s="44"/>
-      <c r="K101" s="44"/>
+      <c r="A101" s="43"/>
+      <c r="B101" s="43"/>
+      <c r="C101" s="43"/>
+      <c r="D101" s="43"/>
+      <c r="E101" s="43"/>
+      <c r="F101" s="43"/>
+      <c r="G101" s="43"/>
+      <c r="H101" s="43"/>
+      <c r="I101" s="43"/>
+      <c r="J101" s="43"/>
+      <c r="K101" s="43"/>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A102" s="44"/>
-      <c r="B102" s="44"/>
-      <c r="C102" s="44"/>
-      <c r="D102" s="44"/>
-      <c r="E102" s="44"/>
-      <c r="F102" s="44"/>
-      <c r="G102" s="44"/>
-      <c r="H102" s="44"/>
-      <c r="I102" s="44"/>
-      <c r="J102" s="44"/>
-      <c r="K102" s="44"/>
+      <c r="A102" s="43"/>
+      <c r="B102" s="43"/>
+      <c r="C102" s="43"/>
+      <c r="D102" s="43"/>
+      <c r="E102" s="43"/>
+      <c r="F102" s="43"/>
+      <c r="G102" s="43"/>
+      <c r="H102" s="43"/>
+      <c r="I102" s="43"/>
+      <c r="J102" s="43"/>
+      <c r="K102" s="43"/>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A103" s="44"/>
-      <c r="B103" s="44"/>
-      <c r="C103" s="44"/>
-      <c r="D103" s="44"/>
-      <c r="E103" s="44"/>
-      <c r="F103" s="44"/>
-      <c r="G103" s="44"/>
-      <c r="H103" s="44"/>
-      <c r="I103" s="44"/>
-      <c r="J103" s="44"/>
-      <c r="K103" s="44"/>
+      <c r="A103" s="43"/>
+      <c r="B103" s="43"/>
+      <c r="C103" s="43"/>
+      <c r="D103" s="43"/>
+      <c r="E103" s="43"/>
+      <c r="F103" s="43"/>
+      <c r="G103" s="43"/>
+      <c r="H103" s="43"/>
+      <c r="I103" s="43"/>
+      <c r="J103" s="43"/>
+      <c r="K103" s="43"/>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A104" s="44"/>
-      <c r="B104" s="44"/>
-      <c r="C104" s="44"/>
-      <c r="D104" s="44"/>
-      <c r="E104" s="44"/>
-      <c r="F104" s="44"/>
-      <c r="G104" s="44"/>
-      <c r="H104" s="44"/>
-      <c r="I104" s="44"/>
-      <c r="J104" s="44"/>
-      <c r="K104" s="44"/>
+      <c r="A104" s="43"/>
+      <c r="B104" s="43"/>
+      <c r="C104" s="43"/>
+      <c r="D104" s="43"/>
+      <c r="E104" s="43"/>
+      <c r="F104" s="43"/>
+      <c r="G104" s="43"/>
+      <c r="H104" s="43"/>
+      <c r="I104" s="43"/>
+      <c r="J104" s="43"/>
+      <c r="K104" s="43"/>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A105" s="44"/>
-      <c r="B105" s="44"/>
-      <c r="C105" s="44"/>
-      <c r="D105" s="44"/>
-      <c r="E105" s="44"/>
-      <c r="F105" s="44"/>
-      <c r="G105" s="44"/>
-      <c r="H105" s="44"/>
-      <c r="I105" s="44"/>
-      <c r="J105" s="44"/>
-      <c r="K105" s="44"/>
+      <c r="A105" s="43"/>
+      <c r="B105" s="43"/>
+      <c r="C105" s="43"/>
+      <c r="D105" s="43"/>
+      <c r="E105" s="43"/>
+      <c r="F105" s="43"/>
+      <c r="G105" s="43"/>
+      <c r="H105" s="43"/>
+      <c r="I105" s="43"/>
+      <c r="J105" s="43"/>
+      <c r="K105" s="43"/>
     </row>
     <row r="106" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="56" t="s">
+      <c r="A106" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="B106" s="56"/>
-      <c r="C106" s="56"/>
-      <c r="D106" s="56"/>
-      <c r="E106" s="56"/>
-      <c r="F106" s="56"/>
-      <c r="G106" s="56"/>
-      <c r="H106" s="56"/>
-      <c r="I106" s="56"/>
-      <c r="J106" s="56"/>
-      <c r="K106" s="56"/>
+      <c r="B106" s="55"/>
+      <c r="C106" s="55"/>
+      <c r="D106" s="55"/>
+      <c r="E106" s="55"/>
+      <c r="F106" s="55"/>
+      <c r="G106" s="55"/>
+      <c r="H106" s="55"/>
+      <c r="I106" s="55"/>
+      <c r="J106" s="55"/>
+      <c r="K106" s="55"/>
     </row>
     <row r="108" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="38" t="s">
@@ -3674,21 +3671,21 @@
       <c r="K113" s="41"/>
     </row>
     <row r="114" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="43" t="s">
+      <c r="A114" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="B114" s="43"/>
-      <c r="C114" s="43"/>
-      <c r="D114" s="43"/>
+      <c r="B114" s="42"/>
+      <c r="C114" s="42"/>
+      <c r="D114" s="42"/>
       <c r="E114" s="31" t="s">
         <v>18</v>
       </c>
       <c r="F114" s="31"/>
-      <c r="G114" s="44" t="s">
+      <c r="G114" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="H114" s="44"/>
-      <c r="I114" s="44"/>
+      <c r="H114" s="43"/>
+      <c r="I114" s="43"/>
       <c r="J114" s="41"/>
       <c r="K114" s="41"/>
     </row>
@@ -3711,55 +3708,55 @@
       <c r="K116" s="41"/>
     </row>
     <row r="117" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A117" s="55" t="s">
+      <c r="A117" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="B117" s="55"/>
-      <c r="C117" s="55"/>
-      <c r="D117" s="55"/>
-      <c r="E117" s="55"/>
-      <c r="F117" s="55"/>
-      <c r="G117" s="55"/>
-      <c r="H117" s="55"/>
-      <c r="I117" s="55"/>
+      <c r="B117" s="54"/>
+      <c r="C117" s="54"/>
+      <c r="D117" s="54"/>
+      <c r="E117" s="54"/>
+      <c r="F117" s="54"/>
+      <c r="G117" s="54"/>
+      <c r="H117" s="54"/>
+      <c r="I117" s="54"/>
       <c r="J117" s="34">
         <v>5</v>
       </c>
       <c r="K117" s="36"/>
     </row>
     <row r="118" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="55" t="s">
+      <c r="A118" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B118" s="55"/>
-      <c r="C118" s="55"/>
-      <c r="D118" s="55"/>
-      <c r="E118" s="55"/>
-      <c r="F118" s="55"/>
-      <c r="G118" s="55"/>
-      <c r="H118" s="55"/>
-      <c r="I118" s="55"/>
-      <c r="J118" s="50">
+      <c r="B118" s="54"/>
+      <c r="C118" s="54"/>
+      <c r="D118" s="54"/>
+      <c r="E118" s="54"/>
+      <c r="F118" s="54"/>
+      <c r="G118" s="54"/>
+      <c r="H118" s="54"/>
+      <c r="I118" s="54"/>
+      <c r="J118" s="49">
         <v>0.98</v>
       </c>
-      <c r="K118" s="51"/>
+      <c r="K118" s="50"/>
     </row>
     <row r="119" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="55" t="s">
+      <c r="A119" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="B119" s="55"/>
-      <c r="C119" s="55"/>
-      <c r="D119" s="55"/>
-      <c r="E119" s="55"/>
-      <c r="F119" s="55"/>
-      <c r="G119" s="55"/>
-      <c r="H119" s="55"/>
-      <c r="I119" s="55"/>
-      <c r="J119" s="50">
+      <c r="B119" s="54"/>
+      <c r="C119" s="54"/>
+      <c r="D119" s="54"/>
+      <c r="E119" s="54"/>
+      <c r="F119" s="54"/>
+      <c r="G119" s="54"/>
+      <c r="H119" s="54"/>
+      <c r="I119" s="54"/>
+      <c r="J119" s="49">
         <v>1.05</v>
       </c>
-      <c r="K119" s="51"/>
+      <c r="K119" s="50"/>
     </row>
     <row r="120" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="34" t="s">
@@ -3773,10 +3770,10 @@
       <c r="G120" s="35"/>
       <c r="H120" s="35"/>
       <c r="I120" s="36"/>
-      <c r="J120" s="50">
+      <c r="J120" s="49">
         <v>1</v>
       </c>
-      <c r="K120" s="51"/>
+      <c r="K120" s="50"/>
     </row>
     <row r="121" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="34" t="s">
@@ -3790,10 +3787,10 @@
       <c r="G121" s="35"/>
       <c r="H121" s="35"/>
       <c r="I121" s="36"/>
-      <c r="J121" s="50">
+      <c r="J121" s="49">
         <v>6</v>
       </c>
-      <c r="K121" s="51"/>
+      <c r="K121" s="50"/>
     </row>
     <row r="122" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="34" t="s">
@@ -3807,10 +3804,10 @@
       <c r="G122" s="35"/>
       <c r="H122" s="35"/>
       <c r="I122" s="36"/>
-      <c r="J122" s="52" t="s">
+      <c r="J122" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="K122" s="53"/>
+      <c r="K122" s="52"/>
     </row>
     <row r="123" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A123" s="34" t="s">
@@ -3824,10 +3821,10 @@
       <c r="G123" s="35"/>
       <c r="H123" s="35"/>
       <c r="I123" s="36"/>
-      <c r="J123" s="50">
+      <c r="J123" s="49">
         <v>2700</v>
       </c>
-      <c r="K123" s="51"/>
+      <c r="K123" s="50"/>
     </row>
     <row r="124" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A124" s="34" t="s">
@@ -3841,10 +3838,10 @@
       <c r="G124" s="35"/>
       <c r="H124" s="35"/>
       <c r="I124" s="36"/>
-      <c r="J124" s="50">
+      <c r="J124" s="49">
         <v>0.16800000000000001</v>
       </c>
-      <c r="K124" s="51"/>
+      <c r="K124" s="50"/>
     </row>
     <row r="125" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A125" s="34" t="s">
@@ -3858,10 +3855,10 @@
       <c r="G125" s="35"/>
       <c r="H125" s="35"/>
       <c r="I125" s="36"/>
-      <c r="J125" s="50">
+      <c r="J125" s="49">
         <v>7.5</v>
       </c>
-      <c r="K125" s="51"/>
+      <c r="K125" s="50"/>
     </row>
     <row r="126" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A126" s="34" t="s">
@@ -3875,10 +3872,10 @@
       <c r="G126" s="35"/>
       <c r="H126" s="35"/>
       <c r="I126" s="36"/>
-      <c r="J126" s="50" t="s">
+      <c r="J126" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="K126" s="51"/>
+      <c r="K126" s="50"/>
     </row>
     <row r="127" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="34" t="s">
@@ -3892,10 +3889,10 @@
       <c r="G127" s="35"/>
       <c r="H127" s="35"/>
       <c r="I127" s="36"/>
-      <c r="J127" s="50">
+      <c r="J127" s="49">
         <v>5</v>
       </c>
-      <c r="K127" s="51"/>
+      <c r="K127" s="50"/>
     </row>
     <row r="128" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="129" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
@@ -3925,10 +3922,10 @@
       <c r="G130" s="35"/>
       <c r="H130" s="35"/>
       <c r="I130" s="36"/>
-      <c r="J130" s="50">
+      <c r="J130" s="49">
         <v>9.5200000000000005E-4</v>
       </c>
-      <c r="K130" s="51"/>
+      <c r="K130" s="50"/>
     </row>
     <row r="131" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="34" t="s">
@@ -3942,10 +3939,10 @@
       <c r="G131" s="35"/>
       <c r="H131" s="35"/>
       <c r="I131" s="36"/>
-      <c r="J131" s="50">
+      <c r="J131" s="49">
         <v>1.2999999999999999E-5</v>
       </c>
-      <c r="K131" s="51"/>
+      <c r="K131" s="50"/>
     </row>
     <row r="132" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="34" t="s">
@@ -3959,10 +3956,10 @@
       <c r="G132" s="35"/>
       <c r="H132" s="35"/>
       <c r="I132" s="36"/>
-      <c r="J132" s="50">
+      <c r="J132" s="49">
         <v>1.9E-2</v>
       </c>
-      <c r="K132" s="51"/>
+      <c r="K132" s="50"/>
     </row>
     <row r="133" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="34" t="s">
@@ -3976,10 +3973,10 @@
       <c r="G133" s="35"/>
       <c r="H133" s="35"/>
       <c r="I133" s="36"/>
-      <c r="J133" s="50">
+      <c r="J133" s="49">
         <v>2500</v>
       </c>
-      <c r="K133" s="51"/>
+      <c r="K133" s="50"/>
     </row>
     <row r="134" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="34" t="s">
@@ -3993,10 +3990,10 @@
       <c r="G134" s="35"/>
       <c r="H134" s="35"/>
       <c r="I134" s="36"/>
-      <c r="J134" s="50">
+      <c r="J134" s="49">
         <v>310</v>
       </c>
-      <c r="K134" s="51"/>
+      <c r="K134" s="50"/>
     </row>
     <row r="135" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="136" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4023,329 +4020,329 @@
     <row r="153" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="154" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="157" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A157" s="44"/>
-      <c r="B157" s="44"/>
-      <c r="C157" s="44"/>
-      <c r="D157" s="44"/>
-      <c r="E157" s="44"/>
-      <c r="F157" s="44"/>
-      <c r="G157" s="44"/>
-      <c r="H157" s="44"/>
-      <c r="I157" s="44"/>
-      <c r="J157" s="44"/>
-      <c r="K157" s="44"/>
+      <c r="A157" s="43"/>
+      <c r="B157" s="43"/>
+      <c r="C157" s="43"/>
+      <c r="D157" s="43"/>
+      <c r="E157" s="43"/>
+      <c r="F157" s="43"/>
+      <c r="G157" s="43"/>
+      <c r="H157" s="43"/>
+      <c r="I157" s="43"/>
+      <c r="J157" s="43"/>
+      <c r="K157" s="43"/>
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A158" s="44"/>
-      <c r="B158" s="44"/>
-      <c r="C158" s="44"/>
-      <c r="D158" s="44"/>
-      <c r="E158" s="44"/>
-      <c r="F158" s="44"/>
-      <c r="G158" s="44"/>
-      <c r="H158" s="44"/>
-      <c r="I158" s="44"/>
-      <c r="J158" s="44"/>
-      <c r="K158" s="44"/>
+      <c r="A158" s="43"/>
+      <c r="B158" s="43"/>
+      <c r="C158" s="43"/>
+      <c r="D158" s="43"/>
+      <c r="E158" s="43"/>
+      <c r="F158" s="43"/>
+      <c r="G158" s="43"/>
+      <c r="H158" s="43"/>
+      <c r="I158" s="43"/>
+      <c r="J158" s="43"/>
+      <c r="K158" s="43"/>
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A159" s="44"/>
-      <c r="B159" s="44"/>
-      <c r="C159" s="44"/>
-      <c r="D159" s="44"/>
-      <c r="E159" s="44"/>
-      <c r="F159" s="44"/>
-      <c r="G159" s="44"/>
-      <c r="H159" s="44"/>
-      <c r="I159" s="44"/>
-      <c r="J159" s="44"/>
-      <c r="K159" s="44"/>
+      <c r="A159" s="43"/>
+      <c r="B159" s="43"/>
+      <c r="C159" s="43"/>
+      <c r="D159" s="43"/>
+      <c r="E159" s="43"/>
+      <c r="F159" s="43"/>
+      <c r="G159" s="43"/>
+      <c r="H159" s="43"/>
+      <c r="I159" s="43"/>
+      <c r="J159" s="43"/>
+      <c r="K159" s="43"/>
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A160" s="44"/>
-      <c r="B160" s="44"/>
-      <c r="C160" s="44"/>
-      <c r="D160" s="44"/>
-      <c r="E160" s="44"/>
-      <c r="F160" s="44"/>
-      <c r="G160" s="44"/>
-      <c r="H160" s="44"/>
-      <c r="I160" s="44"/>
-      <c r="J160" s="44"/>
-      <c r="K160" s="44"/>
+      <c r="A160" s="43"/>
+      <c r="B160" s="43"/>
+      <c r="C160" s="43"/>
+      <c r="D160" s="43"/>
+      <c r="E160" s="43"/>
+      <c r="F160" s="43"/>
+      <c r="G160" s="43"/>
+      <c r="H160" s="43"/>
+      <c r="I160" s="43"/>
+      <c r="J160" s="43"/>
+      <c r="K160" s="43"/>
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A161" s="44"/>
-      <c r="B161" s="44"/>
-      <c r="C161" s="44"/>
-      <c r="D161" s="44"/>
-      <c r="E161" s="44"/>
-      <c r="F161" s="44"/>
-      <c r="G161" s="44"/>
-      <c r="H161" s="44"/>
-      <c r="I161" s="44"/>
-      <c r="J161" s="44"/>
-      <c r="K161" s="44"/>
+      <c r="A161" s="43"/>
+      <c r="B161" s="43"/>
+      <c r="C161" s="43"/>
+      <c r="D161" s="43"/>
+      <c r="E161" s="43"/>
+      <c r="F161" s="43"/>
+      <c r="G161" s="43"/>
+      <c r="H161" s="43"/>
+      <c r="I161" s="43"/>
+      <c r="J161" s="43"/>
+      <c r="K161" s="43"/>
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A162" s="44"/>
-      <c r="B162" s="44"/>
-      <c r="C162" s="44"/>
-      <c r="D162" s="44"/>
-      <c r="E162" s="44"/>
-      <c r="F162" s="44"/>
-      <c r="G162" s="44"/>
-      <c r="H162" s="44"/>
-      <c r="I162" s="44"/>
-      <c r="J162" s="44"/>
-      <c r="K162" s="44"/>
+      <c r="A162" s="43"/>
+      <c r="B162" s="43"/>
+      <c r="C162" s="43"/>
+      <c r="D162" s="43"/>
+      <c r="E162" s="43"/>
+      <c r="F162" s="43"/>
+      <c r="G162" s="43"/>
+      <c r="H162" s="43"/>
+      <c r="I162" s="43"/>
+      <c r="J162" s="43"/>
+      <c r="K162" s="43"/>
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A163" s="44"/>
-      <c r="B163" s="44"/>
-      <c r="C163" s="44"/>
-      <c r="D163" s="44"/>
-      <c r="E163" s="44"/>
-      <c r="F163" s="44"/>
-      <c r="G163" s="44"/>
-      <c r="H163" s="44"/>
-      <c r="I163" s="44"/>
-      <c r="J163" s="44"/>
-      <c r="K163" s="44"/>
+      <c r="A163" s="43"/>
+      <c r="B163" s="43"/>
+      <c r="C163" s="43"/>
+      <c r="D163" s="43"/>
+      <c r="E163" s="43"/>
+      <c r="F163" s="43"/>
+      <c r="G163" s="43"/>
+      <c r="H163" s="43"/>
+      <c r="I163" s="43"/>
+      <c r="J163" s="43"/>
+      <c r="K163" s="43"/>
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A164" s="44"/>
-      <c r="B164" s="44"/>
-      <c r="C164" s="44"/>
-      <c r="D164" s="44"/>
-      <c r="E164" s="44"/>
-      <c r="F164" s="44"/>
-      <c r="G164" s="44"/>
-      <c r="H164" s="44"/>
-      <c r="I164" s="44"/>
-      <c r="J164" s="44"/>
-      <c r="K164" s="44"/>
+      <c r="A164" s="43"/>
+      <c r="B164" s="43"/>
+      <c r="C164" s="43"/>
+      <c r="D164" s="43"/>
+      <c r="E164" s="43"/>
+      <c r="F164" s="43"/>
+      <c r="G164" s="43"/>
+      <c r="H164" s="43"/>
+      <c r="I164" s="43"/>
+      <c r="J164" s="43"/>
+      <c r="K164" s="43"/>
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A165" s="44"/>
-      <c r="B165" s="44"/>
-      <c r="C165" s="44"/>
-      <c r="D165" s="44"/>
-      <c r="E165" s="44"/>
-      <c r="F165" s="44"/>
-      <c r="G165" s="44"/>
-      <c r="H165" s="44"/>
-      <c r="I165" s="44"/>
-      <c r="J165" s="44"/>
-      <c r="K165" s="44"/>
+      <c r="A165" s="43"/>
+      <c r="B165" s="43"/>
+      <c r="C165" s="43"/>
+      <c r="D165" s="43"/>
+      <c r="E165" s="43"/>
+      <c r="F165" s="43"/>
+      <c r="G165" s="43"/>
+      <c r="H165" s="43"/>
+      <c r="I165" s="43"/>
+      <c r="J165" s="43"/>
+      <c r="K165" s="43"/>
     </row>
     <row r="166" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A166" s="44"/>
-      <c r="B166" s="44"/>
-      <c r="C166" s="44"/>
-      <c r="D166" s="44"/>
-      <c r="E166" s="44"/>
-      <c r="F166" s="44"/>
-      <c r="G166" s="44"/>
-      <c r="H166" s="44"/>
-      <c r="I166" s="44"/>
-      <c r="J166" s="44"/>
-      <c r="K166" s="44"/>
+      <c r="A166" s="43"/>
+      <c r="B166" s="43"/>
+      <c r="C166" s="43"/>
+      <c r="D166" s="43"/>
+      <c r="E166" s="43"/>
+      <c r="F166" s="43"/>
+      <c r="G166" s="43"/>
+      <c r="H166" s="43"/>
+      <c r="I166" s="43"/>
+      <c r="J166" s="43"/>
+      <c r="K166" s="43"/>
     </row>
     <row r="167" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A167" s="44"/>
-      <c r="B167" s="44"/>
-      <c r="C167" s="44"/>
-      <c r="D167" s="44"/>
-      <c r="E167" s="44"/>
-      <c r="F167" s="44"/>
-      <c r="G167" s="44"/>
-      <c r="H167" s="44"/>
-      <c r="I167" s="44"/>
-      <c r="J167" s="44"/>
-      <c r="K167" s="44"/>
+      <c r="A167" s="43"/>
+      <c r="B167" s="43"/>
+      <c r="C167" s="43"/>
+      <c r="D167" s="43"/>
+      <c r="E167" s="43"/>
+      <c r="F167" s="43"/>
+      <c r="G167" s="43"/>
+      <c r="H167" s="43"/>
+      <c r="I167" s="43"/>
+      <c r="J167" s="43"/>
+      <c r="K167" s="43"/>
     </row>
     <row r="168" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A168" s="44"/>
-      <c r="B168" s="44"/>
-      <c r="C168" s="44"/>
-      <c r="D168" s="44"/>
-      <c r="E168" s="44"/>
-      <c r="F168" s="44"/>
-      <c r="G168" s="44"/>
-      <c r="H168" s="44"/>
-      <c r="I168" s="44"/>
-      <c r="J168" s="44"/>
-      <c r="K168" s="44"/>
+      <c r="A168" s="43"/>
+      <c r="B168" s="43"/>
+      <c r="C168" s="43"/>
+      <c r="D168" s="43"/>
+      <c r="E168" s="43"/>
+      <c r="F168" s="43"/>
+      <c r="G168" s="43"/>
+      <c r="H168" s="43"/>
+      <c r="I168" s="43"/>
+      <c r="J168" s="43"/>
+      <c r="K168" s="43"/>
     </row>
     <row r="169" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A169" s="44"/>
-      <c r="B169" s="44"/>
-      <c r="C169" s="44"/>
-      <c r="D169" s="44"/>
-      <c r="E169" s="44"/>
-      <c r="F169" s="44"/>
-      <c r="G169" s="44"/>
-      <c r="H169" s="44"/>
-      <c r="I169" s="44"/>
-      <c r="J169" s="44"/>
-      <c r="K169" s="44"/>
+      <c r="A169" s="43"/>
+      <c r="B169" s="43"/>
+      <c r="C169" s="43"/>
+      <c r="D169" s="43"/>
+      <c r="E169" s="43"/>
+      <c r="F169" s="43"/>
+      <c r="G169" s="43"/>
+      <c r="H169" s="43"/>
+      <c r="I169" s="43"/>
+      <c r="J169" s="43"/>
+      <c r="K169" s="43"/>
     </row>
     <row r="170" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A170" s="44"/>
-      <c r="B170" s="44"/>
-      <c r="C170" s="44"/>
-      <c r="D170" s="44"/>
-      <c r="E170" s="44"/>
-      <c r="F170" s="44"/>
-      <c r="G170" s="44"/>
-      <c r="H170" s="44"/>
-      <c r="I170" s="44"/>
-      <c r="J170" s="44"/>
-      <c r="K170" s="44"/>
+      <c r="A170" s="43"/>
+      <c r="B170" s="43"/>
+      <c r="C170" s="43"/>
+      <c r="D170" s="43"/>
+      <c r="E170" s="43"/>
+      <c r="F170" s="43"/>
+      <c r="G170" s="43"/>
+      <c r="H170" s="43"/>
+      <c r="I170" s="43"/>
+      <c r="J170" s="43"/>
+      <c r="K170" s="43"/>
     </row>
     <row r="171" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A171" s="44"/>
-      <c r="B171" s="44"/>
-      <c r="C171" s="44"/>
-      <c r="D171" s="44"/>
-      <c r="E171" s="44"/>
-      <c r="F171" s="44"/>
-      <c r="G171" s="44"/>
-      <c r="H171" s="44"/>
-      <c r="I171" s="44"/>
-      <c r="J171" s="44"/>
-      <c r="K171" s="44"/>
+      <c r="A171" s="43"/>
+      <c r="B171" s="43"/>
+      <c r="C171" s="43"/>
+      <c r="D171" s="43"/>
+      <c r="E171" s="43"/>
+      <c r="F171" s="43"/>
+      <c r="G171" s="43"/>
+      <c r="H171" s="43"/>
+      <c r="I171" s="43"/>
+      <c r="J171" s="43"/>
+      <c r="K171" s="43"/>
     </row>
     <row r="172" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A172" s="44"/>
-      <c r="B172" s="44"/>
-      <c r="C172" s="44"/>
-      <c r="D172" s="44"/>
-      <c r="E172" s="44"/>
-      <c r="F172" s="44"/>
-      <c r="G172" s="44"/>
-      <c r="H172" s="44"/>
-      <c r="I172" s="44"/>
-      <c r="J172" s="44"/>
-      <c r="K172" s="44"/>
+      <c r="A172" s="43"/>
+      <c r="B172" s="43"/>
+      <c r="C172" s="43"/>
+      <c r="D172" s="43"/>
+      <c r="E172" s="43"/>
+      <c r="F172" s="43"/>
+      <c r="G172" s="43"/>
+      <c r="H172" s="43"/>
+      <c r="I172" s="43"/>
+      <c r="J172" s="43"/>
+      <c r="K172" s="43"/>
     </row>
     <row r="173" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A173" s="44"/>
-      <c r="B173" s="44"/>
-      <c r="C173" s="44"/>
-      <c r="D173" s="44"/>
-      <c r="E173" s="44"/>
-      <c r="F173" s="44"/>
-      <c r="G173" s="44"/>
-      <c r="H173" s="44"/>
-      <c r="I173" s="44"/>
-      <c r="J173" s="44"/>
-      <c r="K173" s="44"/>
+      <c r="A173" s="43"/>
+      <c r="B173" s="43"/>
+      <c r="C173" s="43"/>
+      <c r="D173" s="43"/>
+      <c r="E173" s="43"/>
+      <c r="F173" s="43"/>
+      <c r="G173" s="43"/>
+      <c r="H173" s="43"/>
+      <c r="I173" s="43"/>
+      <c r="J173" s="43"/>
+      <c r="K173" s="43"/>
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A174" s="44"/>
-      <c r="B174" s="44"/>
-      <c r="C174" s="44"/>
-      <c r="D174" s="44"/>
-      <c r="E174" s="44"/>
-      <c r="F174" s="44"/>
-      <c r="G174" s="44"/>
-      <c r="H174" s="44"/>
-      <c r="I174" s="44"/>
-      <c r="J174" s="44"/>
-      <c r="K174" s="44"/>
+      <c r="A174" s="43"/>
+      <c r="B174" s="43"/>
+      <c r="C174" s="43"/>
+      <c r="D174" s="43"/>
+      <c r="E174" s="43"/>
+      <c r="F174" s="43"/>
+      <c r="G174" s="43"/>
+      <c r="H174" s="43"/>
+      <c r="I174" s="43"/>
+      <c r="J174" s="43"/>
+      <c r="K174" s="43"/>
     </row>
     <row r="175" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A175" s="44"/>
-      <c r="B175" s="44"/>
-      <c r="C175" s="44"/>
-      <c r="D175" s="44"/>
-      <c r="E175" s="44"/>
-      <c r="F175" s="44"/>
-      <c r="G175" s="44"/>
-      <c r="H175" s="44"/>
-      <c r="I175" s="44"/>
-      <c r="J175" s="44"/>
-      <c r="K175" s="44"/>
+      <c r="A175" s="43"/>
+      <c r="B175" s="43"/>
+      <c r="C175" s="43"/>
+      <c r="D175" s="43"/>
+      <c r="E175" s="43"/>
+      <c r="F175" s="43"/>
+      <c r="G175" s="43"/>
+      <c r="H175" s="43"/>
+      <c r="I175" s="43"/>
+      <c r="J175" s="43"/>
+      <c r="K175" s="43"/>
     </row>
     <row r="176" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A176" s="44"/>
-      <c r="B176" s="44"/>
-      <c r="C176" s="44"/>
-      <c r="D176" s="44"/>
-      <c r="E176" s="44"/>
-      <c r="F176" s="44"/>
-      <c r="G176" s="44"/>
-      <c r="H176" s="44"/>
-      <c r="I176" s="44"/>
-      <c r="J176" s="44"/>
-      <c r="K176" s="44"/>
+      <c r="A176" s="43"/>
+      <c r="B176" s="43"/>
+      <c r="C176" s="43"/>
+      <c r="D176" s="43"/>
+      <c r="E176" s="43"/>
+      <c r="F176" s="43"/>
+      <c r="G176" s="43"/>
+      <c r="H176" s="43"/>
+      <c r="I176" s="43"/>
+      <c r="J176" s="43"/>
+      <c r="K176" s="43"/>
     </row>
     <row r="177" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A177" s="44"/>
-      <c r="B177" s="44"/>
-      <c r="C177" s="44"/>
-      <c r="D177" s="44"/>
-      <c r="E177" s="44"/>
-      <c r="F177" s="44"/>
-      <c r="G177" s="44"/>
-      <c r="H177" s="44"/>
-      <c r="I177" s="44"/>
-      <c r="J177" s="44"/>
-      <c r="K177" s="44"/>
+      <c r="A177" s="43"/>
+      <c r="B177" s="43"/>
+      <c r="C177" s="43"/>
+      <c r="D177" s="43"/>
+      <c r="E177" s="43"/>
+      <c r="F177" s="43"/>
+      <c r="G177" s="43"/>
+      <c r="H177" s="43"/>
+      <c r="I177" s="43"/>
+      <c r="J177" s="43"/>
+      <c r="K177" s="43"/>
     </row>
     <row r="178" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A178" s="44"/>
-      <c r="B178" s="44"/>
-      <c r="C178" s="44"/>
-      <c r="D178" s="44"/>
-      <c r="E178" s="44"/>
-      <c r="F178" s="44"/>
-      <c r="G178" s="44"/>
-      <c r="H178" s="44"/>
-      <c r="I178" s="44"/>
-      <c r="J178" s="44"/>
-      <c r="K178" s="44"/>
+      <c r="A178" s="43"/>
+      <c r="B178" s="43"/>
+      <c r="C178" s="43"/>
+      <c r="D178" s="43"/>
+      <c r="E178" s="43"/>
+      <c r="F178" s="43"/>
+      <c r="G178" s="43"/>
+      <c r="H178" s="43"/>
+      <c r="I178" s="43"/>
+      <c r="J178" s="43"/>
+      <c r="K178" s="43"/>
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A179" s="44"/>
-      <c r="B179" s="44"/>
-      <c r="C179" s="44"/>
-      <c r="D179" s="44"/>
-      <c r="E179" s="44"/>
-      <c r="F179" s="44"/>
-      <c r="G179" s="44"/>
-      <c r="H179" s="44"/>
-      <c r="I179" s="44"/>
-      <c r="J179" s="44"/>
-      <c r="K179" s="44"/>
+      <c r="A179" s="43"/>
+      <c r="B179" s="43"/>
+      <c r="C179" s="43"/>
+      <c r="D179" s="43"/>
+      <c r="E179" s="43"/>
+      <c r="F179" s="43"/>
+      <c r="G179" s="43"/>
+      <c r="H179" s="43"/>
+      <c r="I179" s="43"/>
+      <c r="J179" s="43"/>
+      <c r="K179" s="43"/>
     </row>
     <row r="180" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A180" s="44"/>
-      <c r="B180" s="44"/>
-      <c r="C180" s="44"/>
-      <c r="D180" s="44"/>
-      <c r="E180" s="44"/>
-      <c r="F180" s="44"/>
-      <c r="G180" s="44"/>
-      <c r="H180" s="44"/>
-      <c r="I180" s="44"/>
-      <c r="J180" s="44"/>
-      <c r="K180" s="44"/>
+      <c r="A180" s="43"/>
+      <c r="B180" s="43"/>
+      <c r="C180" s="43"/>
+      <c r="D180" s="43"/>
+      <c r="E180" s="43"/>
+      <c r="F180" s="43"/>
+      <c r="G180" s="43"/>
+      <c r="H180" s="43"/>
+      <c r="I180" s="43"/>
+      <c r="J180" s="43"/>
+      <c r="K180" s="43"/>
     </row>
     <row r="181" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="44"/>
-      <c r="B181" s="44"/>
-      <c r="C181" s="44"/>
-      <c r="D181" s="44"/>
-      <c r="E181" s="44"/>
-      <c r="F181" s="44"/>
-      <c r="G181" s="44"/>
-      <c r="H181" s="44"/>
-      <c r="I181" s="44"/>
-      <c r="J181" s="44"/>
-      <c r="K181" s="44"/>
+      <c r="A181" s="43"/>
+      <c r="B181" s="43"/>
+      <c r="C181" s="43"/>
+      <c r="D181" s="43"/>
+      <c r="E181" s="43"/>
+      <c r="F181" s="43"/>
+      <c r="G181" s="43"/>
+      <c r="H181" s="43"/>
+      <c r="I181" s="43"/>
+      <c r="J181" s="43"/>
+      <c r="K181" s="43"/>
     </row>
     <row r="182" spans="1:11" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A182" s="39" t="s">
@@ -4633,12 +4630,12 @@
       <c r="A210" s="13">
         <v>1</v>
       </c>
-      <c r="B210" s="43" t="s">
+      <c r="B210" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="C210" s="43"/>
-      <c r="D210" s="43"/>
-      <c r="E210" s="43"/>
+      <c r="C210" s="42"/>
+      <c r="D210" s="42"/>
+      <c r="E210" s="42"/>
       <c r="F210" s="25"/>
       <c r="G210" s="26"/>
       <c r="H210" s="25"/>
@@ -4650,12 +4647,12 @@
       <c r="A211" s="13">
         <v>2</v>
       </c>
-      <c r="B211" s="43" t="s">
+      <c r="B211" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="C211" s="43"/>
-      <c r="D211" s="43"/>
-      <c r="E211" s="43"/>
+      <c r="C211" s="42"/>
+      <c r="D211" s="42"/>
+      <c r="E211" s="42"/>
       <c r="F211" s="29"/>
       <c r="G211" s="30"/>
       <c r="H211" s="29"/>
@@ -4667,12 +4664,12 @@
       <c r="A212" s="13">
         <v>3</v>
       </c>
-      <c r="B212" s="43" t="s">
+      <c r="B212" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="C212" s="43"/>
-      <c r="D212" s="43"/>
-      <c r="E212" s="43"/>
+      <c r="C212" s="42"/>
+      <c r="D212" s="42"/>
+      <c r="E212" s="42"/>
       <c r="F212" s="25"/>
       <c r="G212" s="26"/>
       <c r="H212" s="25"/>
@@ -4684,12 +4681,12 @@
       <c r="A213" s="13">
         <v>4</v>
       </c>
-      <c r="B213" s="43" t="s">
+      <c r="B213" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="C213" s="43"/>
-      <c r="D213" s="43"/>
-      <c r="E213" s="43"/>
+      <c r="C213" s="42"/>
+      <c r="D213" s="42"/>
+      <c r="E213" s="42"/>
       <c r="F213" s="25"/>
       <c r="G213" s="26"/>
       <c r="H213" s="25"/>
@@ -4701,12 +4698,12 @@
       <c r="A214" s="13">
         <v>5</v>
       </c>
-      <c r="B214" s="43" t="s">
+      <c r="B214" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="C214" s="43"/>
-      <c r="D214" s="43"/>
-      <c r="E214" s="43"/>
+      <c r="C214" s="42"/>
+      <c r="D214" s="42"/>
+      <c r="E214" s="42"/>
       <c r="F214" s="32"/>
       <c r="G214" s="33"/>
       <c r="H214" s="32"/>
@@ -4718,12 +4715,12 @@
       <c r="A215" s="13">
         <v>6</v>
       </c>
-      <c r="B215" s="43" t="s">
+      <c r="B215" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="C215" s="43"/>
-      <c r="D215" s="43"/>
-      <c r="E215" s="43"/>
+      <c r="C215" s="42"/>
+      <c r="D215" s="42"/>
+      <c r="E215" s="42"/>
       <c r="F215" s="32"/>
       <c r="G215" s="33"/>
       <c r="H215" s="32"/>
@@ -4735,12 +4732,12 @@
       <c r="A216" s="13">
         <v>7</v>
       </c>
-      <c r="B216" s="43" t="s">
+      <c r="B216" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="C216" s="43"/>
-      <c r="D216" s="43"/>
-      <c r="E216" s="43"/>
+      <c r="C216" s="42"/>
+      <c r="D216" s="42"/>
+      <c r="E216" s="42"/>
       <c r="F216" s="28"/>
       <c r="G216" s="28"/>
       <c r="H216" s="28"/>
@@ -4752,12 +4749,12 @@
       <c r="A217" s="13">
         <v>8</v>
       </c>
-      <c r="B217" s="43" t="s">
+      <c r="B217" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="C217" s="43"/>
-      <c r="D217" s="43"/>
-      <c r="E217" s="43"/>
+      <c r="C217" s="42"/>
+      <c r="D217" s="42"/>
+      <c r="E217" s="42"/>
       <c r="F217" s="28"/>
       <c r="G217" s="28"/>
       <c r="H217" s="28"/>
@@ -4769,12 +4766,12 @@
       <c r="A218" s="13">
         <v>9</v>
       </c>
-      <c r="B218" s="43" t="s">
+      <c r="B218" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="C218" s="43"/>
-      <c r="D218" s="43"/>
-      <c r="E218" s="43"/>
+      <c r="C218" s="42"/>
+      <c r="D218" s="42"/>
+      <c r="E218" s="42"/>
       <c r="F218" s="28"/>
       <c r="G218" s="28"/>
       <c r="H218" s="28"/>
@@ -4786,12 +4783,12 @@
       <c r="A219" s="13">
         <v>10</v>
       </c>
-      <c r="B219" s="43" t="s">
+      <c r="B219" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="C219" s="43"/>
-      <c r="D219" s="43"/>
-      <c r="E219" s="43"/>
+      <c r="C219" s="42"/>
+      <c r="D219" s="42"/>
+      <c r="E219" s="42"/>
       <c r="F219" s="27"/>
       <c r="G219" s="27"/>
       <c r="H219" s="27"/>
@@ -4803,12 +4800,12 @@
       <c r="A220" s="13">
         <v>11</v>
       </c>
-      <c r="B220" s="43" t="s">
+      <c r="B220" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="C220" s="43"/>
-      <c r="D220" s="43"/>
-      <c r="E220" s="43"/>
+      <c r="C220" s="42"/>
+      <c r="D220" s="42"/>
+      <c r="E220" s="42"/>
       <c r="F220" s="27"/>
       <c r="G220" s="27"/>
       <c r="H220" s="27"/>
@@ -4820,12 +4817,12 @@
       <c r="A221" s="13">
         <v>12</v>
       </c>
-      <c r="B221" s="43" t="s">
+      <c r="B221" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="C221" s="43"/>
-      <c r="D221" s="43"/>
-      <c r="E221" s="43"/>
+      <c r="C221" s="42"/>
+      <c r="D221" s="42"/>
+      <c r="E221" s="42"/>
       <c r="F221" s="25"/>
       <c r="G221" s="26"/>
       <c r="H221" s="25"/>
@@ -4837,12 +4834,12 @@
       <c r="A222" s="13">
         <v>13</v>
       </c>
-      <c r="B222" s="43" t="s">
+      <c r="B222" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="C222" s="43"/>
-      <c r="D222" s="43"/>
-      <c r="E222" s="43"/>
+      <c r="C222" s="42"/>
+      <c r="D222" s="42"/>
+      <c r="E222" s="42"/>
       <c r="F222" s="25"/>
       <c r="G222" s="26"/>
       <c r="H222" s="25"/>
@@ -4854,12 +4851,12 @@
       <c r="A223" s="13">
         <v>14</v>
       </c>
-      <c r="B223" s="43" t="s">
+      <c r="B223" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C223" s="43"/>
-      <c r="D223" s="43"/>
-      <c r="E223" s="43"/>
+      <c r="C223" s="42"/>
+      <c r="D223" s="42"/>
+      <c r="E223" s="42"/>
       <c r="F223" s="25"/>
       <c r="G223" s="26"/>
       <c r="H223" s="25"/>
@@ -4869,6 +4866,8 @@
     </row>
   </sheetData>
   <mergeCells count="170">
+    <mergeCell ref="J133:K133"/>
+    <mergeCell ref="B21:E21"/>
     <mergeCell ref="A82:K105"/>
     <mergeCell ref="A54:K78"/>
     <mergeCell ref="A157:K181"/>
@@ -4890,6 +4889,12 @@
     <mergeCell ref="H194:I194"/>
     <mergeCell ref="A195:G195"/>
     <mergeCell ref="H195:I195"/>
+    <mergeCell ref="J131:K131"/>
+    <mergeCell ref="J132:K132"/>
+    <mergeCell ref="B212:E212"/>
+    <mergeCell ref="H216:I216"/>
+    <mergeCell ref="H215:I215"/>
+    <mergeCell ref="H214:I214"/>
     <mergeCell ref="A31:K34"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A5:F5"/>
@@ -4910,8 +4915,10 @@
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="J125:K125"/>
+    <mergeCell ref="J126:K126"/>
+    <mergeCell ref="J127:K127"/>
+    <mergeCell ref="J130:K130"/>
     <mergeCell ref="B219:E219"/>
     <mergeCell ref="B220:E220"/>
     <mergeCell ref="B221:E221"/>
@@ -4932,14 +4939,6 @@
     <mergeCell ref="B217:E217"/>
     <mergeCell ref="B209:E209"/>
     <mergeCell ref="B211:E211"/>
-    <mergeCell ref="B212:E212"/>
-    <mergeCell ref="H216:I216"/>
-    <mergeCell ref="H215:I215"/>
-    <mergeCell ref="H214:I214"/>
-    <mergeCell ref="J131:K131"/>
-    <mergeCell ref="J132:K132"/>
-    <mergeCell ref="J133:K133"/>
-    <mergeCell ref="J134:K134"/>
     <mergeCell ref="J116:K116"/>
     <mergeCell ref="J117:K117"/>
     <mergeCell ref="J118:K118"/>
@@ -4949,12 +4948,6 @@
     <mergeCell ref="J122:K122"/>
     <mergeCell ref="J123:K123"/>
     <mergeCell ref="J124:K124"/>
-    <mergeCell ref="J125:K125"/>
-    <mergeCell ref="J126:K126"/>
-    <mergeCell ref="J127:K127"/>
-    <mergeCell ref="J130:K130"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="B21:E21"/>
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="H18:J18"/>
     <mergeCell ref="H19:J19"/>
@@ -4965,6 +4958,9 @@
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B18:E18"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="H16:J16"/>
     <mergeCell ref="A1:L2"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="F10:G10"/>
@@ -5004,6 +5000,7 @@
     <mergeCell ref="A123:I123"/>
     <mergeCell ref="A114:D114"/>
     <mergeCell ref="E114:F114"/>
+    <mergeCell ref="J134:K134"/>
     <mergeCell ref="J211:K211"/>
     <mergeCell ref="J216:K216"/>
     <mergeCell ref="J209:K209"/>
@@ -5063,73 +5060,59 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A61271CF-AC86-4562-8C38-B72111CE1D75}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="65.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="17"/>
+    <col min="1" max="1" width="65.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>90</v>
       </c>
       <c r="B1" s="23"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-    </row>
-    <row r="2" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>91</v>
       </c>
       <c r="B2" s="23"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-    </row>
-    <row r="3" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>92</v>
       </c>
       <c r="B3" s="23"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-    </row>
-    <row r="4" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>93</v>
       </c>
       <c r="B4" s="23"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-    </row>
-    <row r="5" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>94</v>
       </c>
       <c r="B5" s="23"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-    </row>
-    <row r="6" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>79</v>
       </c>
       <c r="B6" s="23"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-    </row>
-    <row r="7" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>95</v>
       </c>
       <c r="B7" s="23"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D7">
@@ -5274,217 +5257,217 @@
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44" t="s">
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44" t="s">
+      <c r="G10" s="43"/>
+      <c r="H10" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44" t="s">
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="44"/>
+      <c r="L10" s="43"/>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>1</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="48" t="s">
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="48"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="44"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>2</v>
       </c>
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="48" t="s">
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="48"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="44"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>3</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="48" t="s">
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="48"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="44"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>4</v>
       </c>
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="48" t="s">
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="48"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="44"/>
-      <c r="L14" s="44"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>5</v>
       </c>
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="48" t="s">
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="48"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="44"/>
-      <c r="L15" s="44"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>6</v>
       </c>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="48" t="s">
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="48"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="44"/>
-      <c r="K16" s="44"/>
-      <c r="L16" s="44"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="43"/>
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>7</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="48" t="s">
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="48"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="44"/>
-      <c r="K17" s="44"/>
-      <c r="L17" s="44"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="43"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>8</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="48" t="s">
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="48"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="44"/>
-      <c r="J18" s="44"/>
-      <c r="K18" s="44"/>
-      <c r="L18" s="44"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="43"/>
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>9</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="48" t="s">
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="48"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
-      <c r="K19" s="44"/>
-      <c r="L19" s="44"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="43"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
       <c r="F21" s="1">
         <v>1000</v>
       </c>
@@ -5587,62 +5570,62 @@
       <c r="L30"/>
     </row>
     <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="54" t="str">
+      <c r="A31" s="53" t="str">
         <f>"Выводы: по сценариям Р90, Р50, Р10 получилось, что с вероятностью 90% начальные геологические запасы газа составят "&amp;C25&amp;" млрд м3, с вероятностью 50% - "&amp;C27&amp;" млрд м3,  с вероятностью 10% - "&amp;C29&amp;" млрд м3"</f>
         <v>Выводы: по сценариям Р90, Р50, Р10 получилось, что с вероятностью 90% начальные геологические запасы газа составят 6655,5 млрд м3, с вероятностью 50% - 8530,8 млрд м3,  с вероятностью 10% - 10406,1 млрд м3</v>
       </c>
-      <c r="B31" s="54"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="54"/>
-      <c r="H31" s="54"/>
-      <c r="I31" s="54"/>
-      <c r="J31" s="54"/>
-      <c r="K31" s="54"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="53"/>
+      <c r="K31" s="53"/>
       <c r="L31"/>
     </row>
     <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="54"/>
-      <c r="B32" s="54"/>
-      <c r="C32" s="54"/>
-      <c r="D32" s="54"/>
-      <c r="E32" s="54"/>
-      <c r="F32" s="54"/>
-      <c r="G32" s="54"/>
-      <c r="H32" s="54"/>
-      <c r="I32" s="54"/>
-      <c r="J32" s="54"/>
-      <c r="K32" s="54"/>
+      <c r="A32" s="53"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="53"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="53"/>
+      <c r="I32" s="53"/>
+      <c r="J32" s="53"/>
+      <c r="K32" s="53"/>
       <c r="L32"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="54"/>
-      <c r="B33" s="54"/>
-      <c r="C33" s="54"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="54"/>
-      <c r="H33" s="54"/>
-      <c r="I33" s="54"/>
-      <c r="J33" s="54"/>
-      <c r="K33" s="54"/>
+      <c r="A33" s="53"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="53"/>
+      <c r="K33" s="53"/>
       <c r="L33"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="54"/>
-      <c r="B34" s="54"/>
-      <c r="C34" s="54"/>
-      <c r="D34" s="54"/>
-      <c r="E34" s="54"/>
-      <c r="F34" s="54"/>
-      <c r="G34" s="54"/>
-      <c r="H34" s="54"/>
-      <c r="I34" s="54"/>
-      <c r="J34" s="54"/>
-      <c r="K34" s="54"/>
+      <c r="A34" s="53"/>
+      <c r="B34" s="53"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="53"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="53"/>
+      <c r="K34" s="53"/>
       <c r="L34"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -6077,44 +6060,44 @@
       <c r="L68"/>
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B69" s="56" t="s">
+      <c r="B69" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="C69" s="56"/>
-      <c r="D69" s="56"/>
-      <c r="E69" s="56"/>
-      <c r="F69" s="56"/>
-      <c r="G69" s="56"/>
-      <c r="H69" s="56"/>
-      <c r="I69" s="56"/>
-      <c r="J69" s="56"/>
-      <c r="K69" s="56"/>
+      <c r="C69" s="55"/>
+      <c r="D69" s="55"/>
+      <c r="E69" s="55"/>
+      <c r="F69" s="55"/>
+      <c r="G69" s="55"/>
+      <c r="H69" s="55"/>
+      <c r="I69" s="55"/>
+      <c r="J69" s="55"/>
+      <c r="K69" s="55"/>
       <c r="L69"/>
     </row>
     <row r="70" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B70" s="56"/>
-      <c r="C70" s="56"/>
-      <c r="D70" s="56"/>
-      <c r="E70" s="56"/>
-      <c r="F70" s="56"/>
-      <c r="G70" s="56"/>
-      <c r="H70" s="56"/>
-      <c r="I70" s="56"/>
-      <c r="J70" s="56"/>
-      <c r="K70" s="56"/>
+      <c r="B70" s="55"/>
+      <c r="C70" s="55"/>
+      <c r="D70" s="55"/>
+      <c r="E70" s="55"/>
+      <c r="F70" s="55"/>
+      <c r="G70" s="55"/>
+      <c r="H70" s="55"/>
+      <c r="I70" s="55"/>
+      <c r="J70" s="55"/>
+      <c r="K70" s="55"/>
       <c r="L70"/>
     </row>
     <row r="71" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B71" s="56"/>
-      <c r="C71" s="56"/>
-      <c r="D71" s="56"/>
-      <c r="E71" s="56"/>
-      <c r="F71" s="56"/>
-      <c r="G71" s="56"/>
-      <c r="H71" s="56"/>
-      <c r="I71" s="56"/>
-      <c r="J71" s="56"/>
-      <c r="K71" s="56"/>
+      <c r="B71" s="55"/>
+      <c r="C71" s="55"/>
+      <c r="D71" s="55"/>
+      <c r="E71" s="55"/>
+      <c r="F71" s="55"/>
+      <c r="G71" s="55"/>
+      <c r="H71" s="55"/>
+      <c r="I71" s="55"/>
+      <c r="J71" s="55"/>
+      <c r="K71" s="55"/>
       <c r="L71"/>
     </row>
     <row r="72" spans="2:12" ht="20.25" x14ac:dyDescent="0.3">
@@ -6274,18 +6257,18 @@
       <c r="L83"/>
     </row>
     <row r="84" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B84" s="56" t="s">
+      <c r="B84" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="C84" s="56"/>
-      <c r="D84" s="56"/>
-      <c r="E84" s="56"/>
-      <c r="F84" s="56"/>
-      <c r="G84" s="56"/>
-      <c r="H84" s="56"/>
-      <c r="I84" s="56"/>
-      <c r="J84" s="56"/>
-      <c r="K84" s="56"/>
+      <c r="C84" s="55"/>
+      <c r="D84" s="55"/>
+      <c r="E84" s="55"/>
+      <c r="F84" s="55"/>
+      <c r="G84" s="55"/>
+      <c r="H84" s="55"/>
+      <c r="I84" s="55"/>
+      <c r="J84" s="55"/>
+      <c r="K84" s="55"/>
       <c r="L84"/>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
@@ -6499,12 +6482,12 @@
       <c r="K101" s="41"/>
     </row>
     <row r="102" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A102" s="43" t="s">
+      <c r="A102" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="B102" s="43"/>
-      <c r="C102" s="43"/>
-      <c r="D102" s="43"/>
+      <c r="B102" s="42"/>
+      <c r="C102" s="42"/>
+      <c r="D102" s="42"/>
       <c r="E102" s="31" t="s">
         <v>18</v>
       </c>
@@ -6533,169 +6516,169 @@
       <c r="K104" s="41"/>
     </row>
     <row r="105" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A105" s="55" t="s">
+      <c r="A105" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="B105" s="55"/>
-      <c r="C105" s="55"/>
-      <c r="D105" s="55"/>
-      <c r="E105" s="55"/>
-      <c r="F105" s="55"/>
-      <c r="G105" s="55"/>
-      <c r="H105" s="55"/>
-      <c r="I105" s="55"/>
+      <c r="B105" s="54"/>
+      <c r="C105" s="54"/>
+      <c r="D105" s="54"/>
+      <c r="E105" s="54"/>
+      <c r="F105" s="54"/>
+      <c r="G105" s="54"/>
+      <c r="H105" s="54"/>
+      <c r="I105" s="54"/>
       <c r="J105" s="34"/>
       <c r="K105" s="36"/>
     </row>
     <row r="106" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A106" s="55" t="s">
+      <c r="A106" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B106" s="55"/>
-      <c r="C106" s="55"/>
-      <c r="D106" s="55"/>
-      <c r="E106" s="55"/>
-      <c r="F106" s="55"/>
-      <c r="G106" s="55"/>
-      <c r="H106" s="55"/>
-      <c r="I106" s="55"/>
-      <c r="J106" s="50"/>
-      <c r="K106" s="51"/>
+      <c r="B106" s="54"/>
+      <c r="C106" s="54"/>
+      <c r="D106" s="54"/>
+      <c r="E106" s="54"/>
+      <c r="F106" s="54"/>
+      <c r="G106" s="54"/>
+      <c r="H106" s="54"/>
+      <c r="I106" s="54"/>
+      <c r="J106" s="49"/>
+      <c r="K106" s="50"/>
     </row>
     <row r="107" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A107" s="55" t="s">
+      <c r="A107" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="B107" s="55"/>
-      <c r="C107" s="55"/>
-      <c r="D107" s="55"/>
-      <c r="E107" s="55"/>
-      <c r="F107" s="55"/>
-      <c r="G107" s="55"/>
-      <c r="H107" s="55"/>
-      <c r="I107" s="55"/>
-      <c r="J107" s="50"/>
-      <c r="K107" s="51"/>
+      <c r="B107" s="54"/>
+      <c r="C107" s="54"/>
+      <c r="D107" s="54"/>
+      <c r="E107" s="54"/>
+      <c r="F107" s="54"/>
+      <c r="G107" s="54"/>
+      <c r="H107" s="54"/>
+      <c r="I107" s="54"/>
+      <c r="J107" s="49"/>
+      <c r="K107" s="50"/>
     </row>
     <row r="108" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A108" s="55" t="s">
+      <c r="A108" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B108" s="55"/>
-      <c r="C108" s="55"/>
-      <c r="D108" s="55"/>
-      <c r="E108" s="55"/>
-      <c r="F108" s="55"/>
-      <c r="G108" s="55"/>
-      <c r="H108" s="55"/>
-      <c r="I108" s="55"/>
-      <c r="J108" s="50"/>
-      <c r="K108" s="51"/>
+      <c r="B108" s="54"/>
+      <c r="C108" s="54"/>
+      <c r="D108" s="54"/>
+      <c r="E108" s="54"/>
+      <c r="F108" s="54"/>
+      <c r="G108" s="54"/>
+      <c r="H108" s="54"/>
+      <c r="I108" s="54"/>
+      <c r="J108" s="49"/>
+      <c r="K108" s="50"/>
     </row>
     <row r="109" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A109" s="55" t="s">
+      <c r="A109" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="B109" s="55"/>
-      <c r="C109" s="55"/>
-      <c r="D109" s="55"/>
-      <c r="E109" s="55"/>
-      <c r="F109" s="55"/>
-      <c r="G109" s="55"/>
-      <c r="H109" s="55"/>
-      <c r="I109" s="55"/>
-      <c r="J109" s="50"/>
-      <c r="K109" s="51"/>
+      <c r="B109" s="54"/>
+      <c r="C109" s="54"/>
+      <c r="D109" s="54"/>
+      <c r="E109" s="54"/>
+      <c r="F109" s="54"/>
+      <c r="G109" s="54"/>
+      <c r="H109" s="54"/>
+      <c r="I109" s="54"/>
+      <c r="J109" s="49"/>
+      <c r="K109" s="50"/>
     </row>
     <row r="110" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A110" s="55" t="s">
+      <c r="A110" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="B110" s="55"/>
-      <c r="C110" s="55"/>
-      <c r="D110" s="55"/>
-      <c r="E110" s="55"/>
-      <c r="F110" s="55"/>
-      <c r="G110" s="55"/>
-      <c r="H110" s="55"/>
-      <c r="I110" s="55"/>
-      <c r="J110" s="50"/>
-      <c r="K110" s="51"/>
+      <c r="B110" s="54"/>
+      <c r="C110" s="54"/>
+      <c r="D110" s="54"/>
+      <c r="E110" s="54"/>
+      <c r="F110" s="54"/>
+      <c r="G110" s="54"/>
+      <c r="H110" s="54"/>
+      <c r="I110" s="54"/>
+      <c r="J110" s="49"/>
+      <c r="K110" s="50"/>
     </row>
     <row r="111" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A111" s="55" t="s">
+      <c r="A111" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="B111" s="55"/>
-      <c r="C111" s="55"/>
-      <c r="D111" s="55"/>
-      <c r="E111" s="55"/>
-      <c r="F111" s="55"/>
-      <c r="G111" s="55"/>
-      <c r="H111" s="55"/>
-      <c r="I111" s="55"/>
-      <c r="J111" s="50"/>
-      <c r="K111" s="51"/>
+      <c r="B111" s="54"/>
+      <c r="C111" s="54"/>
+      <c r="D111" s="54"/>
+      <c r="E111" s="54"/>
+      <c r="F111" s="54"/>
+      <c r="G111" s="54"/>
+      <c r="H111" s="54"/>
+      <c r="I111" s="54"/>
+      <c r="J111" s="49"/>
+      <c r="K111" s="50"/>
     </row>
     <row r="112" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A112" s="55" t="s">
+      <c r="A112" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="B112" s="55"/>
-      <c r="C112" s="55"/>
-      <c r="D112" s="55"/>
-      <c r="E112" s="55"/>
-      <c r="F112" s="55"/>
-      <c r="G112" s="55"/>
-      <c r="H112" s="55"/>
-      <c r="I112" s="55"/>
-      <c r="J112" s="50"/>
-      <c r="K112" s="51"/>
+      <c r="B112" s="54"/>
+      <c r="C112" s="54"/>
+      <c r="D112" s="54"/>
+      <c r="E112" s="54"/>
+      <c r="F112" s="54"/>
+      <c r="G112" s="54"/>
+      <c r="H112" s="54"/>
+      <c r="I112" s="54"/>
+      <c r="J112" s="49"/>
+      <c r="K112" s="50"/>
     </row>
     <row r="113" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A113" s="55" t="s">
+      <c r="A113" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="B113" s="55"/>
-      <c r="C113" s="55"/>
-      <c r="D113" s="55"/>
-      <c r="E113" s="55"/>
-      <c r="F113" s="55"/>
-      <c r="G113" s="55"/>
-      <c r="H113" s="55"/>
-      <c r="I113" s="55"/>
-      <c r="J113" s="50"/>
-      <c r="K113" s="51"/>
+      <c r="B113" s="54"/>
+      <c r="C113" s="54"/>
+      <c r="D113" s="54"/>
+      <c r="E113" s="54"/>
+      <c r="F113" s="54"/>
+      <c r="G113" s="54"/>
+      <c r="H113" s="54"/>
+      <c r="I113" s="54"/>
+      <c r="J113" s="49"/>
+      <c r="K113" s="50"/>
     </row>
     <row r="114" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A114" s="55" t="s">
+      <c r="A114" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="B114" s="55"/>
-      <c r="C114" s="55"/>
-      <c r="D114" s="55"/>
-      <c r="E114" s="55"/>
-      <c r="F114" s="55"/>
-      <c r="G114" s="55"/>
-      <c r="H114" s="55"/>
-      <c r="I114" s="55"/>
-      <c r="J114" s="50"/>
-      <c r="K114" s="51"/>
+      <c r="B114" s="54"/>
+      <c r="C114" s="54"/>
+      <c r="D114" s="54"/>
+      <c r="E114" s="54"/>
+      <c r="F114" s="54"/>
+      <c r="G114" s="54"/>
+      <c r="H114" s="54"/>
+      <c r="I114" s="54"/>
+      <c r="J114" s="49"/>
+      <c r="K114" s="50"/>
     </row>
     <row r="115" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A115" s="55" t="s">
+      <c r="A115" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="B115" s="55"/>
-      <c r="C115" s="55"/>
-      <c r="D115" s="55"/>
-      <c r="E115" s="55"/>
-      <c r="F115" s="55"/>
-      <c r="G115" s="55"/>
-      <c r="H115" s="55"/>
-      <c r="I115" s="55"/>
-      <c r="J115" s="50"/>
-      <c r="K115" s="51"/>
+      <c r="B115" s="54"/>
+      <c r="C115" s="54"/>
+      <c r="D115" s="54"/>
+      <c r="E115" s="54"/>
+      <c r="F115" s="54"/>
+      <c r="G115" s="54"/>
+      <c r="H115" s="54"/>
+      <c r="I115" s="54"/>
+      <c r="J115" s="49"/>
+      <c r="K115" s="50"/>
     </row>
     <row r="117" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A117" s="37" t="s">
@@ -6713,77 +6696,77 @@
       <c r="K117" s="37"/>
     </row>
     <row r="118" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A118" s="55" t="s">
+      <c r="A118" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="B118" s="55"/>
-      <c r="C118" s="55"/>
-      <c r="D118" s="55"/>
-      <c r="E118" s="55"/>
-      <c r="F118" s="55"/>
-      <c r="G118" s="55"/>
-      <c r="H118" s="55"/>
-      <c r="I118" s="55"/>
+      <c r="B118" s="54"/>
+      <c r="C118" s="54"/>
+      <c r="D118" s="54"/>
+      <c r="E118" s="54"/>
+      <c r="F118" s="54"/>
+      <c r="G118" s="54"/>
+      <c r="H118" s="54"/>
+      <c r="I118" s="54"/>
       <c r="J118" s="41"/>
       <c r="K118" s="41"/>
     </row>
     <row r="119" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A119" s="55" t="s">
+      <c r="A119" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="B119" s="55"/>
-      <c r="C119" s="55"/>
-      <c r="D119" s="55"/>
-      <c r="E119" s="55"/>
-      <c r="F119" s="55"/>
-      <c r="G119" s="55"/>
-      <c r="H119" s="55"/>
-      <c r="I119" s="55"/>
+      <c r="B119" s="54"/>
+      <c r="C119" s="54"/>
+      <c r="D119" s="54"/>
+      <c r="E119" s="54"/>
+      <c r="F119" s="54"/>
+      <c r="G119" s="54"/>
+      <c r="H119" s="54"/>
+      <c r="I119" s="54"/>
       <c r="J119" s="41"/>
       <c r="K119" s="41"/>
     </row>
     <row r="120" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A120" s="55" t="s">
+      <c r="A120" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="B120" s="55"/>
-      <c r="C120" s="55"/>
-      <c r="D120" s="55"/>
-      <c r="E120" s="55"/>
-      <c r="F120" s="55"/>
-      <c r="G120" s="55"/>
-      <c r="H120" s="55"/>
-      <c r="I120" s="55"/>
+      <c r="B120" s="54"/>
+      <c r="C120" s="54"/>
+      <c r="D120" s="54"/>
+      <c r="E120" s="54"/>
+      <c r="F120" s="54"/>
+      <c r="G120" s="54"/>
+      <c r="H120" s="54"/>
+      <c r="I120" s="54"/>
       <c r="J120" s="41"/>
       <c r="K120" s="41"/>
     </row>
     <row r="121" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A121" s="55" t="s">
+      <c r="A121" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="B121" s="55"/>
-      <c r="C121" s="55"/>
-      <c r="D121" s="55"/>
-      <c r="E121" s="55"/>
-      <c r="F121" s="55"/>
-      <c r="G121" s="55"/>
-      <c r="H121" s="55"/>
-      <c r="I121" s="55"/>
+      <c r="B121" s="54"/>
+      <c r="C121" s="54"/>
+      <c r="D121" s="54"/>
+      <c r="E121" s="54"/>
+      <c r="F121" s="54"/>
+      <c r="G121" s="54"/>
+      <c r="H121" s="54"/>
+      <c r="I121" s="54"/>
       <c r="J121" s="41"/>
       <c r="K121" s="41"/>
     </row>
     <row r="122" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A122" s="55" t="s">
+      <c r="A122" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="B122" s="55"/>
-      <c r="C122" s="55"/>
-      <c r="D122" s="55"/>
-      <c r="E122" s="55"/>
-      <c r="F122" s="55"/>
-      <c r="G122" s="55"/>
-      <c r="H122" s="55"/>
-      <c r="I122" s="55"/>
+      <c r="B122" s="54"/>
+      <c r="C122" s="54"/>
+      <c r="D122" s="54"/>
+      <c r="E122" s="54"/>
+      <c r="F122" s="54"/>
+      <c r="G122" s="54"/>
+      <c r="H122" s="54"/>
+      <c r="I122" s="54"/>
       <c r="J122" s="41"/>
       <c r="K122" s="41"/>
     </row>
@@ -7019,239 +7002,239 @@
       <c r="A141" s="13">
         <v>1</v>
       </c>
-      <c r="B141" s="43" t="s">
+      <c r="B141" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="C141" s="43"/>
-      <c r="D141" s="43"/>
-      <c r="E141" s="43"/>
+      <c r="C141" s="42"/>
+      <c r="D141" s="42"/>
+      <c r="E141" s="42"/>
       <c r="F141" s="61"/>
       <c r="G141" s="62"/>
-      <c r="H141" s="50"/>
-      <c r="I141" s="51"/>
-      <c r="J141" s="50"/>
-      <c r="K141" s="51"/>
+      <c r="H141" s="49"/>
+      <c r="I141" s="50"/>
+      <c r="J141" s="49"/>
+      <c r="K141" s="50"/>
     </row>
     <row r="142" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="13">
         <v>2</v>
       </c>
-      <c r="B142" s="43" t="s">
+      <c r="B142" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="C142" s="43"/>
-      <c r="D142" s="43"/>
-      <c r="E142" s="43"/>
-      <c r="F142" s="50"/>
-      <c r="G142" s="51"/>
-      <c r="H142" s="50"/>
-      <c r="I142" s="51"/>
-      <c r="J142" s="50"/>
-      <c r="K142" s="51"/>
+      <c r="C142" s="42"/>
+      <c r="D142" s="42"/>
+      <c r="E142" s="42"/>
+      <c r="F142" s="49"/>
+      <c r="G142" s="50"/>
+      <c r="H142" s="49"/>
+      <c r="I142" s="50"/>
+      <c r="J142" s="49"/>
+      <c r="K142" s="50"/>
     </row>
     <row r="143" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="13">
         <v>3</v>
       </c>
-      <c r="B143" s="43" t="s">
+      <c r="B143" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="C143" s="43"/>
-      <c r="D143" s="43"/>
-      <c r="E143" s="43"/>
-      <c r="F143" s="50"/>
-      <c r="G143" s="51"/>
-      <c r="H143" s="50"/>
-      <c r="I143" s="51"/>
-      <c r="J143" s="50"/>
-      <c r="K143" s="51"/>
+      <c r="C143" s="42"/>
+      <c r="D143" s="42"/>
+      <c r="E143" s="42"/>
+      <c r="F143" s="49"/>
+      <c r="G143" s="50"/>
+      <c r="H143" s="49"/>
+      <c r="I143" s="50"/>
+      <c r="J143" s="49"/>
+      <c r="K143" s="50"/>
     </row>
     <row r="144" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="13">
         <v>4</v>
       </c>
-      <c r="B144" s="43" t="s">
+      <c r="B144" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="C144" s="43"/>
-      <c r="D144" s="43"/>
-      <c r="E144" s="43"/>
-      <c r="F144" s="50"/>
-      <c r="G144" s="51"/>
-      <c r="H144" s="50"/>
-      <c r="I144" s="51"/>
-      <c r="J144" s="50"/>
-      <c r="K144" s="51"/>
+      <c r="C144" s="42"/>
+      <c r="D144" s="42"/>
+      <c r="E144" s="42"/>
+      <c r="F144" s="49"/>
+      <c r="G144" s="50"/>
+      <c r="H144" s="49"/>
+      <c r="I144" s="50"/>
+      <c r="J144" s="49"/>
+      <c r="K144" s="50"/>
     </row>
     <row r="145" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="13">
         <v>5</v>
       </c>
-      <c r="B145" s="43" t="s">
+      <c r="B145" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="C145" s="43"/>
-      <c r="D145" s="43"/>
-      <c r="E145" s="43"/>
-      <c r="F145" s="50"/>
-      <c r="G145" s="51"/>
-      <c r="H145" s="50"/>
-      <c r="I145" s="51"/>
-      <c r="J145" s="50"/>
-      <c r="K145" s="51"/>
+      <c r="C145" s="42"/>
+      <c r="D145" s="42"/>
+      <c r="E145" s="42"/>
+      <c r="F145" s="49"/>
+      <c r="G145" s="50"/>
+      <c r="H145" s="49"/>
+      <c r="I145" s="50"/>
+      <c r="J145" s="49"/>
+      <c r="K145" s="50"/>
     </row>
     <row r="146" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="13">
         <v>6</v>
       </c>
-      <c r="B146" s="43" t="s">
+      <c r="B146" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="C146" s="43"/>
-      <c r="D146" s="43"/>
-      <c r="E146" s="43"/>
-      <c r="F146" s="50"/>
-      <c r="G146" s="51"/>
-      <c r="H146" s="50"/>
-      <c r="I146" s="51"/>
-      <c r="J146" s="50"/>
-      <c r="K146" s="51"/>
+      <c r="C146" s="42"/>
+      <c r="D146" s="42"/>
+      <c r="E146" s="42"/>
+      <c r="F146" s="49"/>
+      <c r="G146" s="50"/>
+      <c r="H146" s="49"/>
+      <c r="I146" s="50"/>
+      <c r="J146" s="49"/>
+      <c r="K146" s="50"/>
     </row>
     <row r="147" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="13">
         <v>7</v>
       </c>
-      <c r="B147" s="43" t="s">
+      <c r="B147" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="C147" s="43"/>
-      <c r="D147" s="43"/>
-      <c r="E147" s="43"/>
-      <c r="F147" s="50"/>
-      <c r="G147" s="51"/>
-      <c r="H147" s="50"/>
-      <c r="I147" s="51"/>
-      <c r="J147" s="50"/>
-      <c r="K147" s="51"/>
+      <c r="C147" s="42"/>
+      <c r="D147" s="42"/>
+      <c r="E147" s="42"/>
+      <c r="F147" s="49"/>
+      <c r="G147" s="50"/>
+      <c r="H147" s="49"/>
+      <c r="I147" s="50"/>
+      <c r="J147" s="49"/>
+      <c r="K147" s="50"/>
     </row>
     <row r="148" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="13">
         <v>8</v>
       </c>
-      <c r="B148" s="43" t="s">
+      <c r="B148" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="C148" s="43"/>
-      <c r="D148" s="43"/>
-      <c r="E148" s="43"/>
-      <c r="F148" s="50"/>
-      <c r="G148" s="51"/>
-      <c r="H148" s="50"/>
-      <c r="I148" s="51"/>
-      <c r="J148" s="50"/>
-      <c r="K148" s="51"/>
+      <c r="C148" s="42"/>
+      <c r="D148" s="42"/>
+      <c r="E148" s="42"/>
+      <c r="F148" s="49"/>
+      <c r="G148" s="50"/>
+      <c r="H148" s="49"/>
+      <c r="I148" s="50"/>
+      <c r="J148" s="49"/>
+      <c r="K148" s="50"/>
     </row>
     <row r="149" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="13">
         <v>9</v>
       </c>
-      <c r="B149" s="43" t="s">
+      <c r="B149" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="C149" s="43"/>
-      <c r="D149" s="43"/>
-      <c r="E149" s="43"/>
-      <c r="F149" s="50"/>
-      <c r="G149" s="51"/>
-      <c r="H149" s="50"/>
-      <c r="I149" s="51"/>
-      <c r="J149" s="50"/>
-      <c r="K149" s="51"/>
+      <c r="C149" s="42"/>
+      <c r="D149" s="42"/>
+      <c r="E149" s="42"/>
+      <c r="F149" s="49"/>
+      <c r="G149" s="50"/>
+      <c r="H149" s="49"/>
+      <c r="I149" s="50"/>
+      <c r="J149" s="49"/>
+      <c r="K149" s="50"/>
     </row>
     <row r="150" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="13">
         <v>10</v>
       </c>
-      <c r="B150" s="43" t="s">
+      <c r="B150" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="C150" s="43"/>
-      <c r="D150" s="43"/>
-      <c r="E150" s="43"/>
-      <c r="F150" s="50"/>
-      <c r="G150" s="51"/>
-      <c r="H150" s="50"/>
-      <c r="I150" s="51"/>
-      <c r="J150" s="50"/>
-      <c r="K150" s="51"/>
+      <c r="C150" s="42"/>
+      <c r="D150" s="42"/>
+      <c r="E150" s="42"/>
+      <c r="F150" s="49"/>
+      <c r="G150" s="50"/>
+      <c r="H150" s="49"/>
+      <c r="I150" s="50"/>
+      <c r="J150" s="49"/>
+      <c r="K150" s="50"/>
     </row>
     <row r="151" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="13">
         <v>11</v>
       </c>
-      <c r="B151" s="43" t="s">
+      <c r="B151" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="C151" s="43"/>
-      <c r="D151" s="43"/>
-      <c r="E151" s="43"/>
-      <c r="F151" s="50"/>
-      <c r="G151" s="51"/>
-      <c r="H151" s="50"/>
-      <c r="I151" s="51"/>
-      <c r="J151" s="50"/>
-      <c r="K151" s="51"/>
+      <c r="C151" s="42"/>
+      <c r="D151" s="42"/>
+      <c r="E151" s="42"/>
+      <c r="F151" s="49"/>
+      <c r="G151" s="50"/>
+      <c r="H151" s="49"/>
+      <c r="I151" s="50"/>
+      <c r="J151" s="49"/>
+      <c r="K151" s="50"/>
     </row>
     <row r="152" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="13">
         <v>12</v>
       </c>
-      <c r="B152" s="43" t="s">
+      <c r="B152" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="C152" s="43"/>
-      <c r="D152" s="43"/>
-      <c r="E152" s="43"/>
-      <c r="F152" s="50"/>
-      <c r="G152" s="51"/>
-      <c r="H152" s="50"/>
-      <c r="I152" s="51"/>
-      <c r="J152" s="50"/>
-      <c r="K152" s="51"/>
+      <c r="C152" s="42"/>
+      <c r="D152" s="42"/>
+      <c r="E152" s="42"/>
+      <c r="F152" s="49"/>
+      <c r="G152" s="50"/>
+      <c r="H152" s="49"/>
+      <c r="I152" s="50"/>
+      <c r="J152" s="49"/>
+      <c r="K152" s="50"/>
     </row>
     <row r="153" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="13">
         <v>13</v>
       </c>
-      <c r="B153" s="43" t="s">
+      <c r="B153" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="C153" s="43"/>
-      <c r="D153" s="43"/>
-      <c r="E153" s="43"/>
-      <c r="F153" s="50"/>
-      <c r="G153" s="51"/>
-      <c r="H153" s="50"/>
-      <c r="I153" s="51"/>
-      <c r="J153" s="50"/>
-      <c r="K153" s="51"/>
+      <c r="C153" s="42"/>
+      <c r="D153" s="42"/>
+      <c r="E153" s="42"/>
+      <c r="F153" s="49"/>
+      <c r="G153" s="50"/>
+      <c r="H153" s="49"/>
+      <c r="I153" s="50"/>
+      <c r="J153" s="49"/>
+      <c r="K153" s="50"/>
     </row>
     <row r="154" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="13">
         <v>14</v>
       </c>
-      <c r="B154" s="43" t="s">
+      <c r="B154" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C154" s="43"/>
-      <c r="D154" s="43"/>
-      <c r="E154" s="43"/>
-      <c r="F154" s="50"/>
-      <c r="G154" s="51"/>
-      <c r="H154" s="50"/>
-      <c r="I154" s="51"/>
-      <c r="J154" s="50"/>
-      <c r="K154" s="51"/>
+      <c r="C154" s="42"/>
+      <c r="D154" s="42"/>
+      <c r="E154" s="42"/>
+      <c r="F154" s="49"/>
+      <c r="G154" s="50"/>
+      <c r="H154" s="49"/>
+      <c r="I154" s="50"/>
+      <c r="J154" s="49"/>
+      <c r="K154" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="162">

</xml_diff>